<commit_message>
Day 42, chapter 13 pdfs and world documents
</commit_message>
<xml_diff>
--- a/Chapter_12/testV2.xlsx
+++ b/Chapter_12/testV2.xlsx
@@ -353,7 +353,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD32"/>
+  <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -572,70 +572,242 @@
       </c>
     </row>
     <row r="3" spans="1:30">
-      <c r="A3" s="1" t="s"/>
-      <c r="B3" t="s"/>
-      <c r="C3" t="s"/>
-      <c r="D3" t="s"/>
-      <c r="E3" t="s"/>
-      <c r="F3" t="s"/>
-      <c r="G3" t="s"/>
-      <c r="H3" t="s"/>
-      <c r="I3" t="s"/>
-      <c r="J3" t="s"/>
-      <c r="K3" t="s"/>
-      <c r="L3" t="s"/>
-      <c r="M3" t="s"/>
-      <c r="N3" t="s"/>
-      <c r="O3" t="s"/>
-      <c r="P3" t="s"/>
-      <c r="Q3" t="s"/>
-      <c r="R3" t="s"/>
-      <c r="S3" t="s"/>
-      <c r="T3" t="s"/>
-      <c r="U3" t="s"/>
-      <c r="V3" t="s"/>
-      <c r="W3" t="s"/>
-      <c r="X3" t="s"/>
-      <c r="Y3" t="s"/>
-      <c r="Z3" t="s"/>
-      <c r="AA3" t="s"/>
-      <c r="AB3" t="s"/>
-      <c r="AC3" t="s"/>
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f>A3*B1</f>
+        <v/>
+      </c>
+      <c r="C3">
+        <f>A3*C1</f>
+        <v/>
+      </c>
+      <c r="D3">
+        <f>A3*D1</f>
+        <v/>
+      </c>
+      <c r="E3">
+        <f>A3*E1</f>
+        <v/>
+      </c>
+      <c r="F3">
+        <f>A3*F1</f>
+        <v/>
+      </c>
+      <c r="G3">
+        <f>A3*G1</f>
+        <v/>
+      </c>
+      <c r="H3">
+        <f>A3*H1</f>
+        <v/>
+      </c>
+      <c r="I3">
+        <f>A3*I1</f>
+        <v/>
+      </c>
+      <c r="J3">
+        <f>A3*J1</f>
+        <v/>
+      </c>
+      <c r="K3">
+        <f>A3*K1</f>
+        <v/>
+      </c>
+      <c r="L3">
+        <f>A3*L1</f>
+        <v/>
+      </c>
+      <c r="M3">
+        <f>A3*M1</f>
+        <v/>
+      </c>
+      <c r="N3">
+        <f>A3*N1</f>
+        <v/>
+      </c>
+      <c r="O3">
+        <f>A3*O1</f>
+        <v/>
+      </c>
+      <c r="P3">
+        <f>A3*P1</f>
+        <v/>
+      </c>
+      <c r="Q3">
+        <f>A3*Q1</f>
+        <v/>
+      </c>
+      <c r="R3">
+        <f>A3*R1</f>
+        <v/>
+      </c>
+      <c r="S3">
+        <f>A3*S1</f>
+        <v/>
+      </c>
+      <c r="T3">
+        <f>A3*T1</f>
+        <v/>
+      </c>
+      <c r="U3">
+        <f>A3*U1</f>
+        <v/>
+      </c>
+      <c r="V3">
+        <f>A3*V1</f>
+        <v/>
+      </c>
+      <c r="W3">
+        <f>A3*W1</f>
+        <v/>
+      </c>
+      <c r="X3">
+        <f>A3*X1</f>
+        <v/>
+      </c>
+      <c r="Y3">
+        <f>A3*Y1</f>
+        <v/>
+      </c>
+      <c r="Z3">
+        <f>A3*Z1</f>
+        <v/>
+      </c>
+      <c r="AA3">
+        <f>A3*AA1</f>
+        <v/>
+      </c>
+      <c r="AB3">
+        <f>A3*AB1</f>
+        <v/>
+      </c>
+      <c r="AC3">
+        <f>A3*AC1</f>
+        <v/>
+      </c>
       <c r="AD3">
         <f>A3*AD1</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:30">
-      <c r="A4" s="1" t="s"/>
-      <c r="B4" t="s"/>
-      <c r="C4" t="s"/>
-      <c r="D4" t="s"/>
-      <c r="E4" t="s"/>
-      <c r="F4" t="s"/>
-      <c r="G4" t="s"/>
-      <c r="H4" t="s"/>
-      <c r="I4" t="s"/>
-      <c r="J4" t="s"/>
-      <c r="K4" t="s"/>
-      <c r="L4" t="s"/>
-      <c r="M4" t="s"/>
-      <c r="N4" t="s"/>
-      <c r="O4" t="s"/>
-      <c r="P4" t="s"/>
-      <c r="Q4" t="s"/>
-      <c r="R4" t="s"/>
-      <c r="S4" t="s"/>
-      <c r="T4" t="s"/>
-      <c r="U4" t="s"/>
-      <c r="V4" t="s"/>
-      <c r="W4" t="s"/>
-      <c r="X4" t="s"/>
-      <c r="Y4" t="s"/>
-      <c r="Z4" t="s"/>
-      <c r="AA4" t="s"/>
-      <c r="AB4" t="s"/>
-      <c r="AC4" t="s"/>
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f>A4*B1</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>A4*C1</f>
+        <v/>
+      </c>
+      <c r="D4">
+        <f>A4*D1</f>
+        <v/>
+      </c>
+      <c r="E4">
+        <f>A4*E1</f>
+        <v/>
+      </c>
+      <c r="F4">
+        <f>A4*F1</f>
+        <v/>
+      </c>
+      <c r="G4">
+        <f>A4*G1</f>
+        <v/>
+      </c>
+      <c r="H4">
+        <f>A4*H1</f>
+        <v/>
+      </c>
+      <c r="I4">
+        <f>A4*I1</f>
+        <v/>
+      </c>
+      <c r="J4">
+        <f>A4*J1</f>
+        <v/>
+      </c>
+      <c r="K4">
+        <f>A4*K1</f>
+        <v/>
+      </c>
+      <c r="L4">
+        <f>A4*L1</f>
+        <v/>
+      </c>
+      <c r="M4">
+        <f>A4*M1</f>
+        <v/>
+      </c>
+      <c r="N4">
+        <f>A4*N1</f>
+        <v/>
+      </c>
+      <c r="O4">
+        <f>A4*O1</f>
+        <v/>
+      </c>
+      <c r="P4">
+        <f>A4*P1</f>
+        <v/>
+      </c>
+      <c r="Q4">
+        <f>A4*Q1</f>
+        <v/>
+      </c>
+      <c r="R4">
+        <f>A4*R1</f>
+        <v/>
+      </c>
+      <c r="S4">
+        <f>A4*S1</f>
+        <v/>
+      </c>
+      <c r="T4">
+        <f>A4*T1</f>
+        <v/>
+      </c>
+      <c r="U4">
+        <f>A4*U1</f>
+        <v/>
+      </c>
+      <c r="V4">
+        <f>A4*V1</f>
+        <v/>
+      </c>
+      <c r="W4">
+        <f>A4*W1</f>
+        <v/>
+      </c>
+      <c r="X4">
+        <f>A4*X1</f>
+        <v/>
+      </c>
+      <c r="Y4">
+        <f>A4*Y1</f>
+        <v/>
+      </c>
+      <c r="Z4">
+        <f>A4*Z1</f>
+        <v/>
+      </c>
+      <c r="AA4">
+        <f>A4*AA1</f>
+        <v/>
+      </c>
+      <c r="AB4">
+        <f>A4*AB1</f>
+        <v/>
+      </c>
+      <c r="AC4">
+        <f>A4*AC1</f>
+        <v/>
+      </c>
       <c r="AD4">
         <f>A4*AD1</f>
         <v/>
@@ -643,118 +815,118 @@
     </row>
     <row r="5" spans="1:30">
       <c r="A5" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <f>A3*B1</f>
+        <f>A5*B1</f>
         <v/>
       </c>
       <c r="C5">
-        <f>A3*C1</f>
+        <f>A5*C1</f>
         <v/>
       </c>
       <c r="D5">
-        <f>A3*D1</f>
+        <f>A5*D1</f>
         <v/>
       </c>
       <c r="E5">
-        <f>A3*E1</f>
+        <f>A5*E1</f>
         <v/>
       </c>
       <c r="F5">
-        <f>A3*F1</f>
+        <f>A5*F1</f>
         <v/>
       </c>
       <c r="G5">
-        <f>A3*G1</f>
+        <f>A5*G1</f>
         <v/>
       </c>
       <c r="H5">
-        <f>A3*H1</f>
+        <f>A5*H1</f>
         <v/>
       </c>
       <c r="I5">
-        <f>A3*I1</f>
+        <f>A5*I1</f>
         <v/>
       </c>
       <c r="J5">
-        <f>A3*J1</f>
+        <f>A5*J1</f>
         <v/>
       </c>
       <c r="K5">
-        <f>A3*K1</f>
+        <f>A5*K1</f>
         <v/>
       </c>
       <c r="L5">
-        <f>A3*L1</f>
+        <f>A5*L1</f>
         <v/>
       </c>
       <c r="M5">
-        <f>A3*M1</f>
+        <f>A5*M1</f>
         <v/>
       </c>
       <c r="N5">
-        <f>A3*N1</f>
+        <f>A5*N1</f>
         <v/>
       </c>
       <c r="O5">
-        <f>A3*O1</f>
+        <f>A5*O1</f>
         <v/>
       </c>
       <c r="P5">
-        <f>A3*P1</f>
+        <f>A5*P1</f>
         <v/>
       </c>
       <c r="Q5">
-        <f>A3*Q1</f>
+        <f>A5*Q1</f>
         <v/>
       </c>
       <c r="R5">
-        <f>A3*R1</f>
+        <f>A5*R1</f>
         <v/>
       </c>
       <c r="S5">
-        <f>A3*S1</f>
+        <f>A5*S1</f>
         <v/>
       </c>
       <c r="T5">
-        <f>A3*T1</f>
+        <f>A5*T1</f>
         <v/>
       </c>
       <c r="U5">
-        <f>A3*U1</f>
+        <f>A5*U1</f>
         <v/>
       </c>
       <c r="V5">
-        <f>A3*V1</f>
+        <f>A5*V1</f>
         <v/>
       </c>
       <c r="W5">
-        <f>A3*W1</f>
+        <f>A5*W1</f>
         <v/>
       </c>
       <c r="X5">
-        <f>A3*X1</f>
+        <f>A5*X1</f>
         <v/>
       </c>
       <c r="Y5">
-        <f>A3*Y1</f>
+        <f>A5*Y1</f>
         <v/>
       </c>
       <c r="Z5">
-        <f>A3*Z1</f>
+        <f>A5*Z1</f>
         <v/>
       </c>
       <c r="AA5">
-        <f>A3*AA1</f>
+        <f>A5*AA1</f>
         <v/>
       </c>
       <c r="AB5">
-        <f>A3*AB1</f>
+        <f>A5*AB1</f>
         <v/>
       </c>
       <c r="AC5">
-        <f>A3*AC1</f>
+        <f>A5*AC1</f>
         <v/>
       </c>
       <c r="AD5">
@@ -763,605 +935,175 @@
       </c>
     </row>
     <row r="6" spans="1:30">
-      <c r="A6" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <f>A4*B1</f>
-        <v/>
-      </c>
-      <c r="C6">
-        <f>A4*C1</f>
-        <v/>
-      </c>
-      <c r="D6">
-        <f>A4*D1</f>
-        <v/>
-      </c>
-      <c r="E6">
-        <f>A4*E1</f>
-        <v/>
-      </c>
-      <c r="F6">
-        <f>A4*F1</f>
-        <v/>
-      </c>
-      <c r="G6">
-        <f>A4*G1</f>
-        <v/>
-      </c>
-      <c r="H6">
-        <f>A4*H1</f>
-        <v/>
-      </c>
-      <c r="I6">
-        <f>A4*I1</f>
-        <v/>
-      </c>
-      <c r="J6">
-        <f>A4*J1</f>
-        <v/>
-      </c>
-      <c r="K6">
-        <f>A4*K1</f>
-        <v/>
-      </c>
-      <c r="L6">
-        <f>A4*L1</f>
-        <v/>
-      </c>
-      <c r="M6">
-        <f>A4*M1</f>
-        <v/>
-      </c>
-      <c r="N6">
-        <f>A4*N1</f>
-        <v/>
-      </c>
-      <c r="O6">
-        <f>A4*O1</f>
-        <v/>
-      </c>
-      <c r="P6">
-        <f>A4*P1</f>
-        <v/>
-      </c>
-      <c r="Q6">
-        <f>A4*Q1</f>
-        <v/>
-      </c>
-      <c r="R6">
-        <f>A4*R1</f>
-        <v/>
-      </c>
-      <c r="S6">
-        <f>A4*S1</f>
-        <v/>
-      </c>
-      <c r="T6">
-        <f>A4*T1</f>
-        <v/>
-      </c>
-      <c r="U6">
-        <f>A4*U1</f>
-        <v/>
-      </c>
-      <c r="V6">
-        <f>A4*V1</f>
-        <v/>
-      </c>
-      <c r="W6">
-        <f>A4*W1</f>
-        <v/>
-      </c>
-      <c r="X6">
-        <f>A4*X1</f>
-        <v/>
-      </c>
-      <c r="Y6">
-        <f>A4*Y1</f>
-        <v/>
-      </c>
-      <c r="Z6">
-        <f>A4*Z1</f>
-        <v/>
-      </c>
-      <c r="AA6">
-        <f>A4*AA1</f>
-        <v/>
-      </c>
-      <c r="AB6">
-        <f>A4*AB1</f>
-        <v/>
-      </c>
-      <c r="AC6">
-        <f>A4*AC1</f>
-        <v/>
-      </c>
+      <c r="A6" s="1" t="s"/>
+      <c r="B6" t="s"/>
+      <c r="C6" t="s"/>
+      <c r="D6" t="s"/>
+      <c r="E6" t="s"/>
+      <c r="F6" t="s"/>
+      <c r="G6" t="s"/>
+      <c r="H6" t="s"/>
+      <c r="I6" t="s"/>
+      <c r="J6" t="s"/>
+      <c r="K6" t="s"/>
+      <c r="L6" t="s"/>
+      <c r="M6" t="s"/>
+      <c r="N6" t="s"/>
+      <c r="O6" t="s"/>
+      <c r="P6" t="s"/>
+      <c r="Q6" t="s"/>
+      <c r="R6" t="s"/>
+      <c r="S6" t="s"/>
+      <c r="T6" t="s"/>
+      <c r="U6" t="s"/>
+      <c r="V6" t="s"/>
+      <c r="W6" t="s"/>
+      <c r="X6" t="s"/>
+      <c r="Y6" t="s"/>
+      <c r="Z6" t="s"/>
+      <c r="AA6" t="s"/>
+      <c r="AB6" t="s"/>
+      <c r="AC6" t="s"/>
       <c r="AD6">
         <f>A6*AD1</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:30">
-      <c r="A7" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <f>A5*B1</f>
-        <v/>
-      </c>
-      <c r="C7">
-        <f>A5*C1</f>
-        <v/>
-      </c>
-      <c r="D7">
-        <f>A5*D1</f>
-        <v/>
-      </c>
-      <c r="E7">
-        <f>A5*E1</f>
-        <v/>
-      </c>
-      <c r="F7">
-        <f>A5*F1</f>
-        <v/>
-      </c>
-      <c r="G7">
-        <f>A5*G1</f>
-        <v/>
-      </c>
-      <c r="H7">
-        <f>A5*H1</f>
-        <v/>
-      </c>
-      <c r="I7">
-        <f>A5*I1</f>
-        <v/>
-      </c>
-      <c r="J7">
-        <f>A5*J1</f>
-        <v/>
-      </c>
-      <c r="K7">
-        <f>A5*K1</f>
-        <v/>
-      </c>
-      <c r="L7">
-        <f>A5*L1</f>
-        <v/>
-      </c>
-      <c r="M7">
-        <f>A5*M1</f>
-        <v/>
-      </c>
-      <c r="N7">
-        <f>A5*N1</f>
-        <v/>
-      </c>
-      <c r="O7">
-        <f>A5*O1</f>
-        <v/>
-      </c>
-      <c r="P7">
-        <f>A5*P1</f>
-        <v/>
-      </c>
-      <c r="Q7">
-        <f>A5*Q1</f>
-        <v/>
-      </c>
-      <c r="R7">
-        <f>A5*R1</f>
-        <v/>
-      </c>
-      <c r="S7">
-        <f>A5*S1</f>
-        <v/>
-      </c>
-      <c r="T7">
-        <f>A5*T1</f>
-        <v/>
-      </c>
-      <c r="U7">
-        <f>A5*U1</f>
-        <v/>
-      </c>
-      <c r="V7">
-        <f>A5*V1</f>
-        <v/>
-      </c>
-      <c r="W7">
-        <f>A5*W1</f>
-        <v/>
-      </c>
-      <c r="X7">
-        <f>A5*X1</f>
-        <v/>
-      </c>
-      <c r="Y7">
-        <f>A5*Y1</f>
-        <v/>
-      </c>
-      <c r="Z7">
-        <f>A5*Z1</f>
-        <v/>
-      </c>
-      <c r="AA7">
-        <f>A5*AA1</f>
-        <v/>
-      </c>
-      <c r="AB7">
-        <f>A5*AB1</f>
-        <v/>
-      </c>
-      <c r="AC7">
-        <f>A5*AC1</f>
-        <v/>
-      </c>
+      <c r="A7" s="1" t="s"/>
+      <c r="B7" t="s"/>
+      <c r="C7" t="s"/>
+      <c r="D7" t="s"/>
+      <c r="E7" t="s"/>
+      <c r="F7" t="s"/>
+      <c r="G7" t="s"/>
+      <c r="H7" t="s"/>
+      <c r="I7" t="s"/>
+      <c r="J7" t="s"/>
+      <c r="K7" t="s"/>
+      <c r="L7" t="s"/>
+      <c r="M7" t="s"/>
+      <c r="N7" t="s"/>
+      <c r="O7" t="s"/>
+      <c r="P7" t="s"/>
+      <c r="Q7" t="s"/>
+      <c r="R7" t="s"/>
+      <c r="S7" t="s"/>
+      <c r="T7" t="s"/>
+      <c r="U7" t="s"/>
+      <c r="V7" t="s"/>
+      <c r="W7" t="s"/>
+      <c r="X7" t="s"/>
+      <c r="Y7" t="s"/>
+      <c r="Z7" t="s"/>
+      <c r="AA7" t="s"/>
+      <c r="AB7" t="s"/>
+      <c r="AC7" t="s"/>
       <c r="AD7">
         <f>A7*AD1</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:30">
-      <c r="A8" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <f>A6*B1</f>
-        <v/>
-      </c>
-      <c r="C8">
-        <f>A6*C1</f>
-        <v/>
-      </c>
-      <c r="D8">
-        <f>A6*D1</f>
-        <v/>
-      </c>
-      <c r="E8">
-        <f>A6*E1</f>
-        <v/>
-      </c>
-      <c r="F8">
-        <f>A6*F1</f>
-        <v/>
-      </c>
-      <c r="G8">
-        <f>A6*G1</f>
-        <v/>
-      </c>
-      <c r="H8">
-        <f>A6*H1</f>
-        <v/>
-      </c>
-      <c r="I8">
-        <f>A6*I1</f>
-        <v/>
-      </c>
-      <c r="J8">
-        <f>A6*J1</f>
-        <v/>
-      </c>
-      <c r="K8">
-        <f>A6*K1</f>
-        <v/>
-      </c>
-      <c r="L8">
-        <f>A6*L1</f>
-        <v/>
-      </c>
-      <c r="M8">
-        <f>A6*M1</f>
-        <v/>
-      </c>
-      <c r="N8">
-        <f>A6*N1</f>
-        <v/>
-      </c>
-      <c r="O8">
-        <f>A6*O1</f>
-        <v/>
-      </c>
-      <c r="P8">
-        <f>A6*P1</f>
-        <v/>
-      </c>
-      <c r="Q8">
-        <f>A6*Q1</f>
-        <v/>
-      </c>
-      <c r="R8">
-        <f>A6*R1</f>
-        <v/>
-      </c>
-      <c r="S8">
-        <f>A6*S1</f>
-        <v/>
-      </c>
-      <c r="T8">
-        <f>A6*T1</f>
-        <v/>
-      </c>
-      <c r="U8">
-        <f>A6*U1</f>
-        <v/>
-      </c>
-      <c r="V8">
-        <f>A6*V1</f>
-        <v/>
-      </c>
-      <c r="W8">
-        <f>A6*W1</f>
-        <v/>
-      </c>
-      <c r="X8">
-        <f>A6*X1</f>
-        <v/>
-      </c>
-      <c r="Y8">
-        <f>A6*Y1</f>
-        <v/>
-      </c>
-      <c r="Z8">
-        <f>A6*Z1</f>
-        <v/>
-      </c>
-      <c r="AA8">
-        <f>A6*AA1</f>
-        <v/>
-      </c>
-      <c r="AB8">
-        <f>A6*AB1</f>
-        <v/>
-      </c>
-      <c r="AC8">
-        <f>A6*AC1</f>
-        <v/>
-      </c>
+      <c r="A8" s="1" t="s"/>
+      <c r="B8" t="s"/>
+      <c r="C8" t="s"/>
+      <c r="D8" t="s"/>
+      <c r="E8" t="s"/>
+      <c r="F8" t="s"/>
+      <c r="G8" t="s"/>
+      <c r="H8" t="s"/>
+      <c r="I8" t="s"/>
+      <c r="J8" t="s"/>
+      <c r="K8" t="s"/>
+      <c r="L8" t="s"/>
+      <c r="M8" t="s"/>
+      <c r="N8" t="s"/>
+      <c r="O8" t="s"/>
+      <c r="P8" t="s"/>
+      <c r="Q8" t="s"/>
+      <c r="R8" t="s"/>
+      <c r="S8" t="s"/>
+      <c r="T8" t="s"/>
+      <c r="U8" t="s"/>
+      <c r="V8" t="s"/>
+      <c r="W8" t="s"/>
+      <c r="X8" t="s"/>
+      <c r="Y8" t="s"/>
+      <c r="Z8" t="s"/>
+      <c r="AA8" t="s"/>
+      <c r="AB8" t="s"/>
+      <c r="AC8" t="s"/>
       <c r="AD8">
         <f>A8*AD1</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:30">
-      <c r="A9" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <f>A7*B1</f>
-        <v/>
-      </c>
-      <c r="C9">
-        <f>A7*C1</f>
-        <v/>
-      </c>
-      <c r="D9">
-        <f>A7*D1</f>
-        <v/>
-      </c>
-      <c r="E9">
-        <f>A7*E1</f>
-        <v/>
-      </c>
-      <c r="F9">
-        <f>A7*F1</f>
-        <v/>
-      </c>
-      <c r="G9">
-        <f>A7*G1</f>
-        <v/>
-      </c>
-      <c r="H9">
-        <f>A7*H1</f>
-        <v/>
-      </c>
-      <c r="I9">
-        <f>A7*I1</f>
-        <v/>
-      </c>
-      <c r="J9">
-        <f>A7*J1</f>
-        <v/>
-      </c>
-      <c r="K9">
-        <f>A7*K1</f>
-        <v/>
-      </c>
-      <c r="L9">
-        <f>A7*L1</f>
-        <v/>
-      </c>
-      <c r="M9">
-        <f>A7*M1</f>
-        <v/>
-      </c>
-      <c r="N9">
-        <f>A7*N1</f>
-        <v/>
-      </c>
-      <c r="O9">
-        <f>A7*O1</f>
-        <v/>
-      </c>
-      <c r="P9">
-        <f>A7*P1</f>
-        <v/>
-      </c>
-      <c r="Q9">
-        <f>A7*Q1</f>
-        <v/>
-      </c>
-      <c r="R9">
-        <f>A7*R1</f>
-        <v/>
-      </c>
-      <c r="S9">
-        <f>A7*S1</f>
-        <v/>
-      </c>
-      <c r="T9">
-        <f>A7*T1</f>
-        <v/>
-      </c>
-      <c r="U9">
-        <f>A7*U1</f>
-        <v/>
-      </c>
-      <c r="V9">
-        <f>A7*V1</f>
-        <v/>
-      </c>
-      <c r="W9">
-        <f>A7*W1</f>
-        <v/>
-      </c>
-      <c r="X9">
-        <f>A7*X1</f>
-        <v/>
-      </c>
-      <c r="Y9">
-        <f>A7*Y1</f>
-        <v/>
-      </c>
-      <c r="Z9">
-        <f>A7*Z1</f>
-        <v/>
-      </c>
-      <c r="AA9">
-        <f>A7*AA1</f>
-        <v/>
-      </c>
-      <c r="AB9">
-        <f>A7*AB1</f>
-        <v/>
-      </c>
-      <c r="AC9">
-        <f>A7*AC1</f>
-        <v/>
-      </c>
+      <c r="A9" s="1" t="s"/>
+      <c r="B9" t="s"/>
+      <c r="C9" t="s"/>
+      <c r="D9" t="s"/>
+      <c r="E9" t="s"/>
+      <c r="F9" t="s"/>
+      <c r="G9" t="s"/>
+      <c r="H9" t="s"/>
+      <c r="I9" t="s"/>
+      <c r="J9" t="s"/>
+      <c r="K9" t="s"/>
+      <c r="L9" t="s"/>
+      <c r="M9" t="s"/>
+      <c r="N9" t="s"/>
+      <c r="O9" t="s"/>
+      <c r="P9" t="s"/>
+      <c r="Q9" t="s"/>
+      <c r="R9" t="s"/>
+      <c r="S9" t="s"/>
+      <c r="T9" t="s"/>
+      <c r="U9" t="s"/>
+      <c r="V9" t="s"/>
+      <c r="W9" t="s"/>
+      <c r="X9" t="s"/>
+      <c r="Y9" t="s"/>
+      <c r="Z9" t="s"/>
+      <c r="AA9" t="s"/>
+      <c r="AB9" t="s"/>
+      <c r="AC9" t="s"/>
       <c r="AD9">
         <f>A9*AD1</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:30">
-      <c r="A10" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <f>A8*B1</f>
-        <v/>
-      </c>
-      <c r="C10">
-        <f>A8*C1</f>
-        <v/>
-      </c>
-      <c r="D10">
-        <f>A8*D1</f>
-        <v/>
-      </c>
-      <c r="E10">
-        <f>A8*E1</f>
-        <v/>
-      </c>
-      <c r="F10">
-        <f>A8*F1</f>
-        <v/>
-      </c>
-      <c r="G10">
-        <f>A8*G1</f>
-        <v/>
-      </c>
-      <c r="H10">
-        <f>A8*H1</f>
-        <v/>
-      </c>
-      <c r="I10">
-        <f>A8*I1</f>
-        <v/>
-      </c>
-      <c r="J10">
-        <f>A8*J1</f>
-        <v/>
-      </c>
-      <c r="K10">
-        <f>A8*K1</f>
-        <v/>
-      </c>
-      <c r="L10">
-        <f>A8*L1</f>
-        <v/>
-      </c>
-      <c r="M10">
-        <f>A8*M1</f>
-        <v/>
-      </c>
-      <c r="N10">
-        <f>A8*N1</f>
-        <v/>
-      </c>
-      <c r="O10">
-        <f>A8*O1</f>
-        <v/>
-      </c>
-      <c r="P10">
-        <f>A8*P1</f>
-        <v/>
-      </c>
-      <c r="Q10">
-        <f>A8*Q1</f>
-        <v/>
-      </c>
-      <c r="R10">
-        <f>A8*R1</f>
-        <v/>
-      </c>
-      <c r="S10">
-        <f>A8*S1</f>
-        <v/>
-      </c>
-      <c r="T10">
-        <f>A8*T1</f>
-        <v/>
-      </c>
-      <c r="U10">
-        <f>A8*U1</f>
-        <v/>
-      </c>
-      <c r="V10">
-        <f>A8*V1</f>
-        <v/>
-      </c>
-      <c r="W10">
-        <f>A8*W1</f>
-        <v/>
-      </c>
-      <c r="X10">
-        <f>A8*X1</f>
-        <v/>
-      </c>
-      <c r="Y10">
-        <f>A8*Y1</f>
-        <v/>
-      </c>
-      <c r="Z10">
-        <f>A8*Z1</f>
-        <v/>
-      </c>
-      <c r="AA10">
-        <f>A8*AA1</f>
-        <v/>
-      </c>
-      <c r="AB10">
-        <f>A8*AB1</f>
-        <v/>
-      </c>
-      <c r="AC10">
-        <f>A8*AC1</f>
-        <v/>
-      </c>
+      <c r="A10" s="1" t="s"/>
+      <c r="B10" t="s"/>
+      <c r="C10" t="s"/>
+      <c r="D10" t="s"/>
+      <c r="E10" t="s"/>
+      <c r="F10" t="s"/>
+      <c r="G10" t="s"/>
+      <c r="H10" t="s"/>
+      <c r="I10" t="s"/>
+      <c r="J10" t="s"/>
+      <c r="K10" t="s"/>
+      <c r="L10" t="s"/>
+      <c r="M10" t="s"/>
+      <c r="N10" t="s"/>
+      <c r="O10" t="s"/>
+      <c r="P10" t="s"/>
+      <c r="Q10" t="s"/>
+      <c r="R10" t="s"/>
+      <c r="S10" t="s"/>
+      <c r="T10" t="s"/>
+      <c r="U10" t="s"/>
+      <c r="V10" t="s"/>
+      <c r="W10" t="s"/>
+      <c r="X10" t="s"/>
+      <c r="Y10" t="s"/>
+      <c r="Z10" t="s"/>
+      <c r="AA10" t="s"/>
+      <c r="AB10" t="s"/>
+      <c r="AC10" t="s"/>
       <c r="AD10">
         <f>A10*AD1</f>
         <v/>
@@ -1369,118 +1111,118 @@
     </row>
     <row r="11" spans="1:30">
       <c r="A11" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <f>A9*B1</f>
+        <f>A6*B1</f>
         <v/>
       </c>
       <c r="C11">
-        <f>A9*C1</f>
+        <f>A6*C1</f>
         <v/>
       </c>
       <c r="D11">
-        <f>A9*D1</f>
+        <f>A6*D1</f>
         <v/>
       </c>
       <c r="E11">
-        <f>A9*E1</f>
+        <f>A6*E1</f>
         <v/>
       </c>
       <c r="F11">
-        <f>A9*F1</f>
+        <f>A6*F1</f>
         <v/>
       </c>
       <c r="G11">
-        <f>A9*G1</f>
+        <f>A6*G1</f>
         <v/>
       </c>
       <c r="H11">
-        <f>A9*H1</f>
+        <f>A6*H1</f>
         <v/>
       </c>
       <c r="I11">
-        <f>A9*I1</f>
+        <f>A6*I1</f>
         <v/>
       </c>
       <c r="J11">
-        <f>A9*J1</f>
+        <f>A6*J1</f>
         <v/>
       </c>
       <c r="K11">
-        <f>A9*K1</f>
+        <f>A6*K1</f>
         <v/>
       </c>
       <c r="L11">
-        <f>A9*L1</f>
+        <f>A6*L1</f>
         <v/>
       </c>
       <c r="M11">
-        <f>A9*M1</f>
+        <f>A6*M1</f>
         <v/>
       </c>
       <c r="N11">
-        <f>A9*N1</f>
+        <f>A6*N1</f>
         <v/>
       </c>
       <c r="O11">
-        <f>A9*O1</f>
+        <f>A6*O1</f>
         <v/>
       </c>
       <c r="P11">
-        <f>A9*P1</f>
+        <f>A6*P1</f>
         <v/>
       </c>
       <c r="Q11">
-        <f>A9*Q1</f>
+        <f>A6*Q1</f>
         <v/>
       </c>
       <c r="R11">
-        <f>A9*R1</f>
+        <f>A6*R1</f>
         <v/>
       </c>
       <c r="S11">
-        <f>A9*S1</f>
+        <f>A6*S1</f>
         <v/>
       </c>
       <c r="T11">
-        <f>A9*T1</f>
+        <f>A6*T1</f>
         <v/>
       </c>
       <c r="U11">
-        <f>A9*U1</f>
+        <f>A6*U1</f>
         <v/>
       </c>
       <c r="V11">
-        <f>A9*V1</f>
+        <f>A6*V1</f>
         <v/>
       </c>
       <c r="W11">
-        <f>A9*W1</f>
+        <f>A6*W1</f>
         <v/>
       </c>
       <c r="X11">
-        <f>A9*X1</f>
+        <f>A6*X1</f>
         <v/>
       </c>
       <c r="Y11">
-        <f>A9*Y1</f>
+        <f>A6*Y1</f>
         <v/>
       </c>
       <c r="Z11">
-        <f>A9*Z1</f>
+        <f>A6*Z1</f>
         <v/>
       </c>
       <c r="AA11">
-        <f>A9*AA1</f>
+        <f>A6*AA1</f>
         <v/>
       </c>
       <c r="AB11">
-        <f>A9*AB1</f>
+        <f>A6*AB1</f>
         <v/>
       </c>
       <c r="AC11">
-        <f>A9*AC1</f>
+        <f>A6*AC1</f>
         <v/>
       </c>
       <c r="AD11">
@@ -1490,118 +1232,118 @@
     </row>
     <row r="12" spans="1:30">
       <c r="A12" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B12">
-        <f>A10*B1</f>
+        <f>A7*B1</f>
         <v/>
       </c>
       <c r="C12">
-        <f>A10*C1</f>
+        <f>A7*C1</f>
         <v/>
       </c>
       <c r="D12">
-        <f>A10*D1</f>
+        <f>A7*D1</f>
         <v/>
       </c>
       <c r="E12">
-        <f>A10*E1</f>
+        <f>A7*E1</f>
         <v/>
       </c>
       <c r="F12">
-        <f>A10*F1</f>
+        <f>A7*F1</f>
         <v/>
       </c>
       <c r="G12">
-        <f>A10*G1</f>
+        <f>A7*G1</f>
         <v/>
       </c>
       <c r="H12">
-        <f>A10*H1</f>
+        <f>A7*H1</f>
         <v/>
       </c>
       <c r="I12">
-        <f>A10*I1</f>
+        <f>A7*I1</f>
         <v/>
       </c>
       <c r="J12">
-        <f>A10*J1</f>
+        <f>A7*J1</f>
         <v/>
       </c>
       <c r="K12">
-        <f>A10*K1</f>
+        <f>A7*K1</f>
         <v/>
       </c>
       <c r="L12">
-        <f>A10*L1</f>
+        <f>A7*L1</f>
         <v/>
       </c>
       <c r="M12">
-        <f>A10*M1</f>
+        <f>A7*M1</f>
         <v/>
       </c>
       <c r="N12">
-        <f>A10*N1</f>
+        <f>A7*N1</f>
         <v/>
       </c>
       <c r="O12">
-        <f>A10*O1</f>
+        <f>A7*O1</f>
         <v/>
       </c>
       <c r="P12">
-        <f>A10*P1</f>
+        <f>A7*P1</f>
         <v/>
       </c>
       <c r="Q12">
-        <f>A10*Q1</f>
+        <f>A7*Q1</f>
         <v/>
       </c>
       <c r="R12">
-        <f>A10*R1</f>
+        <f>A7*R1</f>
         <v/>
       </c>
       <c r="S12">
-        <f>A10*S1</f>
+        <f>A7*S1</f>
         <v/>
       </c>
       <c r="T12">
-        <f>A10*T1</f>
+        <f>A7*T1</f>
         <v/>
       </c>
       <c r="U12">
-        <f>A10*U1</f>
+        <f>A7*U1</f>
         <v/>
       </c>
       <c r="V12">
-        <f>A10*V1</f>
+        <f>A7*V1</f>
         <v/>
       </c>
       <c r="W12">
-        <f>A10*W1</f>
+        <f>A7*W1</f>
         <v/>
       </c>
       <c r="X12">
-        <f>A10*X1</f>
+        <f>A7*X1</f>
         <v/>
       </c>
       <c r="Y12">
-        <f>A10*Y1</f>
+        <f>A7*Y1</f>
         <v/>
       </c>
       <c r="Z12">
-        <f>A10*Z1</f>
+        <f>A7*Z1</f>
         <v/>
       </c>
       <c r="AA12">
-        <f>A10*AA1</f>
+        <f>A7*AA1</f>
         <v/>
       </c>
       <c r="AB12">
-        <f>A10*AB1</f>
+        <f>A7*AB1</f>
         <v/>
       </c>
       <c r="AC12">
-        <f>A10*AC1</f>
+        <f>A7*AC1</f>
         <v/>
       </c>
       <c r="AD12">
@@ -1611,118 +1353,118 @@
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="1" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B13">
-        <f>A11*B1</f>
+        <f>A8*B1</f>
         <v/>
       </c>
       <c r="C13">
-        <f>A11*C1</f>
+        <f>A8*C1</f>
         <v/>
       </c>
       <c r="D13">
-        <f>A11*D1</f>
+        <f>A8*D1</f>
         <v/>
       </c>
       <c r="E13">
-        <f>A11*E1</f>
+        <f>A8*E1</f>
         <v/>
       </c>
       <c r="F13">
-        <f>A11*F1</f>
+        <f>A8*F1</f>
         <v/>
       </c>
       <c r="G13">
-        <f>A11*G1</f>
+        <f>A8*G1</f>
         <v/>
       </c>
       <c r="H13">
-        <f>A11*H1</f>
+        <f>A8*H1</f>
         <v/>
       </c>
       <c r="I13">
-        <f>A11*I1</f>
+        <f>A8*I1</f>
         <v/>
       </c>
       <c r="J13">
-        <f>A11*J1</f>
+        <f>A8*J1</f>
         <v/>
       </c>
       <c r="K13">
-        <f>A11*K1</f>
+        <f>A8*K1</f>
         <v/>
       </c>
       <c r="L13">
-        <f>A11*L1</f>
+        <f>A8*L1</f>
         <v/>
       </c>
       <c r="M13">
-        <f>A11*M1</f>
+        <f>A8*M1</f>
         <v/>
       </c>
       <c r="N13">
-        <f>A11*N1</f>
+        <f>A8*N1</f>
         <v/>
       </c>
       <c r="O13">
-        <f>A11*O1</f>
+        <f>A8*O1</f>
         <v/>
       </c>
       <c r="P13">
-        <f>A11*P1</f>
+        <f>A8*P1</f>
         <v/>
       </c>
       <c r="Q13">
-        <f>A11*Q1</f>
+        <f>A8*Q1</f>
         <v/>
       </c>
       <c r="R13">
-        <f>A11*R1</f>
+        <f>A8*R1</f>
         <v/>
       </c>
       <c r="S13">
-        <f>A11*S1</f>
+        <f>A8*S1</f>
         <v/>
       </c>
       <c r="T13">
-        <f>A11*T1</f>
+        <f>A8*T1</f>
         <v/>
       </c>
       <c r="U13">
-        <f>A11*U1</f>
+        <f>A8*U1</f>
         <v/>
       </c>
       <c r="V13">
-        <f>A11*V1</f>
+        <f>A8*V1</f>
         <v/>
       </c>
       <c r="W13">
-        <f>A11*W1</f>
+        <f>A8*W1</f>
         <v/>
       </c>
       <c r="X13">
-        <f>A11*X1</f>
+        <f>A8*X1</f>
         <v/>
       </c>
       <c r="Y13">
-        <f>A11*Y1</f>
+        <f>A8*Y1</f>
         <v/>
       </c>
       <c r="Z13">
-        <f>A11*Z1</f>
+        <f>A8*Z1</f>
         <v/>
       </c>
       <c r="AA13">
-        <f>A11*AA1</f>
+        <f>A8*AA1</f>
         <v/>
       </c>
       <c r="AB13">
-        <f>A11*AB1</f>
+        <f>A8*AB1</f>
         <v/>
       </c>
       <c r="AC13">
-        <f>A11*AC1</f>
+        <f>A8*AC1</f>
         <v/>
       </c>
       <c r="AD13">
@@ -1732,118 +1474,118 @@
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="1" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B14">
-        <f>A12*B1</f>
+        <f>A9*B1</f>
         <v/>
       </c>
       <c r="C14">
-        <f>A12*C1</f>
+        <f>A9*C1</f>
         <v/>
       </c>
       <c r="D14">
-        <f>A12*D1</f>
+        <f>A9*D1</f>
         <v/>
       </c>
       <c r="E14">
-        <f>A12*E1</f>
+        <f>A9*E1</f>
         <v/>
       </c>
       <c r="F14">
-        <f>A12*F1</f>
+        <f>A9*F1</f>
         <v/>
       </c>
       <c r="G14">
-        <f>A12*G1</f>
+        <f>A9*G1</f>
         <v/>
       </c>
       <c r="H14">
-        <f>A12*H1</f>
+        <f>A9*H1</f>
         <v/>
       </c>
       <c r="I14">
-        <f>A12*I1</f>
+        <f>A9*I1</f>
         <v/>
       </c>
       <c r="J14">
-        <f>A12*J1</f>
+        <f>A9*J1</f>
         <v/>
       </c>
       <c r="K14">
-        <f>A12*K1</f>
+        <f>A9*K1</f>
         <v/>
       </c>
       <c r="L14">
-        <f>A12*L1</f>
+        <f>A9*L1</f>
         <v/>
       </c>
       <c r="M14">
-        <f>A12*M1</f>
+        <f>A9*M1</f>
         <v/>
       </c>
       <c r="N14">
-        <f>A12*N1</f>
+        <f>A9*N1</f>
         <v/>
       </c>
       <c r="O14">
-        <f>A12*O1</f>
+        <f>A9*O1</f>
         <v/>
       </c>
       <c r="P14">
-        <f>A12*P1</f>
+        <f>A9*P1</f>
         <v/>
       </c>
       <c r="Q14">
-        <f>A12*Q1</f>
+        <f>A9*Q1</f>
         <v/>
       </c>
       <c r="R14">
-        <f>A12*R1</f>
+        <f>A9*R1</f>
         <v/>
       </c>
       <c r="S14">
-        <f>A12*S1</f>
+        <f>A9*S1</f>
         <v/>
       </c>
       <c r="T14">
-        <f>A12*T1</f>
+        <f>A9*T1</f>
         <v/>
       </c>
       <c r="U14">
-        <f>A12*U1</f>
+        <f>A9*U1</f>
         <v/>
       </c>
       <c r="V14">
-        <f>A12*V1</f>
+        <f>A9*V1</f>
         <v/>
       </c>
       <c r="W14">
-        <f>A12*W1</f>
+        <f>A9*W1</f>
         <v/>
       </c>
       <c r="X14">
-        <f>A12*X1</f>
+        <f>A9*X1</f>
         <v/>
       </c>
       <c r="Y14">
-        <f>A12*Y1</f>
+        <f>A9*Y1</f>
         <v/>
       </c>
       <c r="Z14">
-        <f>A12*Z1</f>
+        <f>A9*Z1</f>
         <v/>
       </c>
       <c r="AA14">
-        <f>A12*AA1</f>
+        <f>A9*AA1</f>
         <v/>
       </c>
       <c r="AB14">
-        <f>A12*AB1</f>
+        <f>A9*AB1</f>
         <v/>
       </c>
       <c r="AC14">
-        <f>A12*AC1</f>
+        <f>A9*AC1</f>
         <v/>
       </c>
       <c r="AD14">
@@ -1853,118 +1595,118 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="1" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B15">
-        <f>A13*B1</f>
+        <f>A10*B1</f>
         <v/>
       </c>
       <c r="C15">
-        <f>A13*C1</f>
+        <f>A10*C1</f>
         <v/>
       </c>
       <c r="D15">
-        <f>A13*D1</f>
+        <f>A10*D1</f>
         <v/>
       </c>
       <c r="E15">
-        <f>A13*E1</f>
+        <f>A10*E1</f>
         <v/>
       </c>
       <c r="F15">
-        <f>A13*F1</f>
+        <f>A10*F1</f>
         <v/>
       </c>
       <c r="G15">
-        <f>A13*G1</f>
+        <f>A10*G1</f>
         <v/>
       </c>
       <c r="H15">
-        <f>A13*H1</f>
+        <f>A10*H1</f>
         <v/>
       </c>
       <c r="I15">
-        <f>A13*I1</f>
+        <f>A10*I1</f>
         <v/>
       </c>
       <c r="J15">
-        <f>A13*J1</f>
+        <f>A10*J1</f>
         <v/>
       </c>
       <c r="K15">
-        <f>A13*K1</f>
+        <f>A10*K1</f>
         <v/>
       </c>
       <c r="L15">
-        <f>A13*L1</f>
+        <f>A10*L1</f>
         <v/>
       </c>
       <c r="M15">
-        <f>A13*M1</f>
+        <f>A10*M1</f>
         <v/>
       </c>
       <c r="N15">
-        <f>A13*N1</f>
+        <f>A10*N1</f>
         <v/>
       </c>
       <c r="O15">
-        <f>A13*O1</f>
+        <f>A10*O1</f>
         <v/>
       </c>
       <c r="P15">
-        <f>A13*P1</f>
+        <f>A10*P1</f>
         <v/>
       </c>
       <c r="Q15">
-        <f>A13*Q1</f>
+        <f>A10*Q1</f>
         <v/>
       </c>
       <c r="R15">
-        <f>A13*R1</f>
+        <f>A10*R1</f>
         <v/>
       </c>
       <c r="S15">
-        <f>A13*S1</f>
+        <f>A10*S1</f>
         <v/>
       </c>
       <c r="T15">
-        <f>A13*T1</f>
+        <f>A10*T1</f>
         <v/>
       </c>
       <c r="U15">
-        <f>A13*U1</f>
+        <f>A10*U1</f>
         <v/>
       </c>
       <c r="V15">
-        <f>A13*V1</f>
+        <f>A10*V1</f>
         <v/>
       </c>
       <c r="W15">
-        <f>A13*W1</f>
+        <f>A10*W1</f>
         <v/>
       </c>
       <c r="X15">
-        <f>A13*X1</f>
+        <f>A10*X1</f>
         <v/>
       </c>
       <c r="Y15">
-        <f>A13*Y1</f>
+        <f>A10*Y1</f>
         <v/>
       </c>
       <c r="Z15">
-        <f>A13*Z1</f>
+        <f>A10*Z1</f>
         <v/>
       </c>
       <c r="AA15">
-        <f>A13*AA1</f>
+        <f>A10*AA1</f>
         <v/>
       </c>
       <c r="AB15">
-        <f>A13*AB1</f>
+        <f>A10*AB1</f>
         <v/>
       </c>
       <c r="AC15">
-        <f>A13*AC1</f>
+        <f>A10*AC1</f>
         <v/>
       </c>
       <c r="AD15">
@@ -1974,118 +1716,118 @@
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="1" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B16">
-        <f>A14*B1</f>
+        <f>A11*B1</f>
         <v/>
       </c>
       <c r="C16">
-        <f>A14*C1</f>
+        <f>A11*C1</f>
         <v/>
       </c>
       <c r="D16">
-        <f>A14*D1</f>
+        <f>A11*D1</f>
         <v/>
       </c>
       <c r="E16">
-        <f>A14*E1</f>
+        <f>A11*E1</f>
         <v/>
       </c>
       <c r="F16">
-        <f>A14*F1</f>
+        <f>A11*F1</f>
         <v/>
       </c>
       <c r="G16">
-        <f>A14*G1</f>
+        <f>A11*G1</f>
         <v/>
       </c>
       <c r="H16">
-        <f>A14*H1</f>
+        <f>A11*H1</f>
         <v/>
       </c>
       <c r="I16">
-        <f>A14*I1</f>
+        <f>A11*I1</f>
         <v/>
       </c>
       <c r="J16">
-        <f>A14*J1</f>
+        <f>A11*J1</f>
         <v/>
       </c>
       <c r="K16">
-        <f>A14*K1</f>
+        <f>A11*K1</f>
         <v/>
       </c>
       <c r="L16">
-        <f>A14*L1</f>
+        <f>A11*L1</f>
         <v/>
       </c>
       <c r="M16">
-        <f>A14*M1</f>
+        <f>A11*M1</f>
         <v/>
       </c>
       <c r="N16">
-        <f>A14*N1</f>
+        <f>A11*N1</f>
         <v/>
       </c>
       <c r="O16">
-        <f>A14*O1</f>
+        <f>A11*O1</f>
         <v/>
       </c>
       <c r="P16">
-        <f>A14*P1</f>
+        <f>A11*P1</f>
         <v/>
       </c>
       <c r="Q16">
-        <f>A14*Q1</f>
+        <f>A11*Q1</f>
         <v/>
       </c>
       <c r="R16">
-        <f>A14*R1</f>
+        <f>A11*R1</f>
         <v/>
       </c>
       <c r="S16">
-        <f>A14*S1</f>
+        <f>A11*S1</f>
         <v/>
       </c>
       <c r="T16">
-        <f>A14*T1</f>
+        <f>A11*T1</f>
         <v/>
       </c>
       <c r="U16">
-        <f>A14*U1</f>
+        <f>A11*U1</f>
         <v/>
       </c>
       <c r="V16">
-        <f>A14*V1</f>
+        <f>A11*V1</f>
         <v/>
       </c>
       <c r="W16">
-        <f>A14*W1</f>
+        <f>A11*W1</f>
         <v/>
       </c>
       <c r="X16">
-        <f>A14*X1</f>
+        <f>A11*X1</f>
         <v/>
       </c>
       <c r="Y16">
-        <f>A14*Y1</f>
+        <f>A11*Y1</f>
         <v/>
       </c>
       <c r="Z16">
-        <f>A14*Z1</f>
+        <f>A11*Z1</f>
         <v/>
       </c>
       <c r="AA16">
-        <f>A14*AA1</f>
+        <f>A11*AA1</f>
         <v/>
       </c>
       <c r="AB16">
-        <f>A14*AB1</f>
+        <f>A11*AB1</f>
         <v/>
       </c>
       <c r="AC16">
-        <f>A14*AC1</f>
+        <f>A11*AC1</f>
         <v/>
       </c>
       <c r="AD16">
@@ -2095,118 +1837,118 @@
     </row>
     <row r="17" spans="1:30">
       <c r="A17" s="1" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B17">
-        <f>A15*B1</f>
+        <f>A12*B1</f>
         <v/>
       </c>
       <c r="C17">
-        <f>A15*C1</f>
+        <f>A12*C1</f>
         <v/>
       </c>
       <c r="D17">
-        <f>A15*D1</f>
+        <f>A12*D1</f>
         <v/>
       </c>
       <c r="E17">
-        <f>A15*E1</f>
+        <f>A12*E1</f>
         <v/>
       </c>
       <c r="F17">
-        <f>A15*F1</f>
+        <f>A12*F1</f>
         <v/>
       </c>
       <c r="G17">
-        <f>A15*G1</f>
+        <f>A12*G1</f>
         <v/>
       </c>
       <c r="H17">
-        <f>A15*H1</f>
+        <f>A12*H1</f>
         <v/>
       </c>
       <c r="I17">
-        <f>A15*I1</f>
+        <f>A12*I1</f>
         <v/>
       </c>
       <c r="J17">
-        <f>A15*J1</f>
+        <f>A12*J1</f>
         <v/>
       </c>
       <c r="K17">
-        <f>A15*K1</f>
+        <f>A12*K1</f>
         <v/>
       </c>
       <c r="L17">
-        <f>A15*L1</f>
+        <f>A12*L1</f>
         <v/>
       </c>
       <c r="M17">
-        <f>A15*M1</f>
+        <f>A12*M1</f>
         <v/>
       </c>
       <c r="N17">
-        <f>A15*N1</f>
+        <f>A12*N1</f>
         <v/>
       </c>
       <c r="O17">
-        <f>A15*O1</f>
+        <f>A12*O1</f>
         <v/>
       </c>
       <c r="P17">
-        <f>A15*P1</f>
+        <f>A12*P1</f>
         <v/>
       </c>
       <c r="Q17">
-        <f>A15*Q1</f>
+        <f>A12*Q1</f>
         <v/>
       </c>
       <c r="R17">
-        <f>A15*R1</f>
+        <f>A12*R1</f>
         <v/>
       </c>
       <c r="S17">
-        <f>A15*S1</f>
+        <f>A12*S1</f>
         <v/>
       </c>
       <c r="T17">
-        <f>A15*T1</f>
+        <f>A12*T1</f>
         <v/>
       </c>
       <c r="U17">
-        <f>A15*U1</f>
+        <f>A12*U1</f>
         <v/>
       </c>
       <c r="V17">
-        <f>A15*V1</f>
+        <f>A12*V1</f>
         <v/>
       </c>
       <c r="W17">
-        <f>A15*W1</f>
+        <f>A12*W1</f>
         <v/>
       </c>
       <c r="X17">
-        <f>A15*X1</f>
+        <f>A12*X1</f>
         <v/>
       </c>
       <c r="Y17">
-        <f>A15*Y1</f>
+        <f>A12*Y1</f>
         <v/>
       </c>
       <c r="Z17">
-        <f>A15*Z1</f>
+        <f>A12*Z1</f>
         <v/>
       </c>
       <c r="AA17">
-        <f>A15*AA1</f>
+        <f>A12*AA1</f>
         <v/>
       </c>
       <c r="AB17">
-        <f>A15*AB1</f>
+        <f>A12*AB1</f>
         <v/>
       </c>
       <c r="AC17">
-        <f>A15*AC1</f>
+        <f>A12*AC1</f>
         <v/>
       </c>
       <c r="AD17">
@@ -2216,118 +1958,118 @@
     </row>
     <row r="18" spans="1:30">
       <c r="A18" s="1" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B18">
-        <f>A16*B1</f>
+        <f>A13*B1</f>
         <v/>
       </c>
       <c r="C18">
-        <f>A16*C1</f>
+        <f>A13*C1</f>
         <v/>
       </c>
       <c r="D18">
-        <f>A16*D1</f>
+        <f>A13*D1</f>
         <v/>
       </c>
       <c r="E18">
-        <f>A16*E1</f>
+        <f>A13*E1</f>
         <v/>
       </c>
       <c r="F18">
-        <f>A16*F1</f>
+        <f>A13*F1</f>
         <v/>
       </c>
       <c r="G18">
-        <f>A16*G1</f>
+        <f>A13*G1</f>
         <v/>
       </c>
       <c r="H18">
-        <f>A16*H1</f>
+        <f>A13*H1</f>
         <v/>
       </c>
       <c r="I18">
-        <f>A16*I1</f>
+        <f>A13*I1</f>
         <v/>
       </c>
       <c r="J18">
-        <f>A16*J1</f>
+        <f>A13*J1</f>
         <v/>
       </c>
       <c r="K18">
-        <f>A16*K1</f>
+        <f>A13*K1</f>
         <v/>
       </c>
       <c r="L18">
-        <f>A16*L1</f>
+        <f>A13*L1</f>
         <v/>
       </c>
       <c r="M18">
-        <f>A16*M1</f>
+        <f>A13*M1</f>
         <v/>
       </c>
       <c r="N18">
-        <f>A16*N1</f>
+        <f>A13*N1</f>
         <v/>
       </c>
       <c r="O18">
-        <f>A16*O1</f>
+        <f>A13*O1</f>
         <v/>
       </c>
       <c r="P18">
-        <f>A16*P1</f>
+        <f>A13*P1</f>
         <v/>
       </c>
       <c r="Q18">
-        <f>A16*Q1</f>
+        <f>A13*Q1</f>
         <v/>
       </c>
       <c r="R18">
-        <f>A16*R1</f>
+        <f>A13*R1</f>
         <v/>
       </c>
       <c r="S18">
-        <f>A16*S1</f>
+        <f>A13*S1</f>
         <v/>
       </c>
       <c r="T18">
-        <f>A16*T1</f>
+        <f>A13*T1</f>
         <v/>
       </c>
       <c r="U18">
-        <f>A16*U1</f>
+        <f>A13*U1</f>
         <v/>
       </c>
       <c r="V18">
-        <f>A16*V1</f>
+        <f>A13*V1</f>
         <v/>
       </c>
       <c r="W18">
-        <f>A16*W1</f>
+        <f>A13*W1</f>
         <v/>
       </c>
       <c r="X18">
-        <f>A16*X1</f>
+        <f>A13*X1</f>
         <v/>
       </c>
       <c r="Y18">
-        <f>A16*Y1</f>
+        <f>A13*Y1</f>
         <v/>
       </c>
       <c r="Z18">
-        <f>A16*Z1</f>
+        <f>A13*Z1</f>
         <v/>
       </c>
       <c r="AA18">
-        <f>A16*AA1</f>
+        <f>A13*AA1</f>
         <v/>
       </c>
       <c r="AB18">
-        <f>A16*AB1</f>
+        <f>A13*AB1</f>
         <v/>
       </c>
       <c r="AC18">
-        <f>A16*AC1</f>
+        <f>A13*AC1</f>
         <v/>
       </c>
       <c r="AD18">
@@ -2337,118 +2079,118 @@
     </row>
     <row r="19" spans="1:30">
       <c r="A19" s="1" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B19">
-        <f>A17*B1</f>
+        <f>A14*B1</f>
         <v/>
       </c>
       <c r="C19">
-        <f>A17*C1</f>
+        <f>A14*C1</f>
         <v/>
       </c>
       <c r="D19">
-        <f>A17*D1</f>
+        <f>A14*D1</f>
         <v/>
       </c>
       <c r="E19">
-        <f>A17*E1</f>
+        <f>A14*E1</f>
         <v/>
       </c>
       <c r="F19">
-        <f>A17*F1</f>
+        <f>A14*F1</f>
         <v/>
       </c>
       <c r="G19">
-        <f>A17*G1</f>
+        <f>A14*G1</f>
         <v/>
       </c>
       <c r="H19">
-        <f>A17*H1</f>
+        <f>A14*H1</f>
         <v/>
       </c>
       <c r="I19">
-        <f>A17*I1</f>
+        <f>A14*I1</f>
         <v/>
       </c>
       <c r="J19">
-        <f>A17*J1</f>
+        <f>A14*J1</f>
         <v/>
       </c>
       <c r="K19">
-        <f>A17*K1</f>
+        <f>A14*K1</f>
         <v/>
       </c>
       <c r="L19">
-        <f>A17*L1</f>
+        <f>A14*L1</f>
         <v/>
       </c>
       <c r="M19">
-        <f>A17*M1</f>
+        <f>A14*M1</f>
         <v/>
       </c>
       <c r="N19">
-        <f>A17*N1</f>
+        <f>A14*N1</f>
         <v/>
       </c>
       <c r="O19">
-        <f>A17*O1</f>
+        <f>A14*O1</f>
         <v/>
       </c>
       <c r="P19">
-        <f>A17*P1</f>
+        <f>A14*P1</f>
         <v/>
       </c>
       <c r="Q19">
-        <f>A17*Q1</f>
+        <f>A14*Q1</f>
         <v/>
       </c>
       <c r="R19">
-        <f>A17*R1</f>
+        <f>A14*R1</f>
         <v/>
       </c>
       <c r="S19">
-        <f>A17*S1</f>
+        <f>A14*S1</f>
         <v/>
       </c>
       <c r="T19">
-        <f>A17*T1</f>
+        <f>A14*T1</f>
         <v/>
       </c>
       <c r="U19">
-        <f>A17*U1</f>
+        <f>A14*U1</f>
         <v/>
       </c>
       <c r="V19">
-        <f>A17*V1</f>
+        <f>A14*V1</f>
         <v/>
       </c>
       <c r="W19">
-        <f>A17*W1</f>
+        <f>A14*W1</f>
         <v/>
       </c>
       <c r="X19">
-        <f>A17*X1</f>
+        <f>A14*X1</f>
         <v/>
       </c>
       <c r="Y19">
-        <f>A17*Y1</f>
+        <f>A14*Y1</f>
         <v/>
       </c>
       <c r="Z19">
-        <f>A17*Z1</f>
+        <f>A14*Z1</f>
         <v/>
       </c>
       <c r="AA19">
-        <f>A17*AA1</f>
+        <f>A14*AA1</f>
         <v/>
       </c>
       <c r="AB19">
-        <f>A17*AB1</f>
+        <f>A14*AB1</f>
         <v/>
       </c>
       <c r="AC19">
-        <f>A17*AC1</f>
+        <f>A14*AC1</f>
         <v/>
       </c>
       <c r="AD19">
@@ -2458,118 +2200,118 @@
     </row>
     <row r="20" spans="1:30">
       <c r="A20" s="1" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B20">
-        <f>A18*B1</f>
+        <f>A15*B1</f>
         <v/>
       </c>
       <c r="C20">
-        <f>A18*C1</f>
+        <f>A15*C1</f>
         <v/>
       </c>
       <c r="D20">
-        <f>A18*D1</f>
+        <f>A15*D1</f>
         <v/>
       </c>
       <c r="E20">
-        <f>A18*E1</f>
+        <f>A15*E1</f>
         <v/>
       </c>
       <c r="F20">
-        <f>A18*F1</f>
+        <f>A15*F1</f>
         <v/>
       </c>
       <c r="G20">
-        <f>A18*G1</f>
+        <f>A15*G1</f>
         <v/>
       </c>
       <c r="H20">
-        <f>A18*H1</f>
+        <f>A15*H1</f>
         <v/>
       </c>
       <c r="I20">
-        <f>A18*I1</f>
+        <f>A15*I1</f>
         <v/>
       </c>
       <c r="J20">
-        <f>A18*J1</f>
+        <f>A15*J1</f>
         <v/>
       </c>
       <c r="K20">
-        <f>A18*K1</f>
+        <f>A15*K1</f>
         <v/>
       </c>
       <c r="L20">
-        <f>A18*L1</f>
+        <f>A15*L1</f>
         <v/>
       </c>
       <c r="M20">
-        <f>A18*M1</f>
+        <f>A15*M1</f>
         <v/>
       </c>
       <c r="N20">
-        <f>A18*N1</f>
+        <f>A15*N1</f>
         <v/>
       </c>
       <c r="O20">
-        <f>A18*O1</f>
+        <f>A15*O1</f>
         <v/>
       </c>
       <c r="P20">
-        <f>A18*P1</f>
+        <f>A15*P1</f>
         <v/>
       </c>
       <c r="Q20">
-        <f>A18*Q1</f>
+        <f>A15*Q1</f>
         <v/>
       </c>
       <c r="R20">
-        <f>A18*R1</f>
+        <f>A15*R1</f>
         <v/>
       </c>
       <c r="S20">
-        <f>A18*S1</f>
+        <f>A15*S1</f>
         <v/>
       </c>
       <c r="T20">
-        <f>A18*T1</f>
+        <f>A15*T1</f>
         <v/>
       </c>
       <c r="U20">
-        <f>A18*U1</f>
+        <f>A15*U1</f>
         <v/>
       </c>
       <c r="V20">
-        <f>A18*V1</f>
+        <f>A15*V1</f>
         <v/>
       </c>
       <c r="W20">
-        <f>A18*W1</f>
+        <f>A15*W1</f>
         <v/>
       </c>
       <c r="X20">
-        <f>A18*X1</f>
+        <f>A15*X1</f>
         <v/>
       </c>
       <c r="Y20">
-        <f>A18*Y1</f>
+        <f>A15*Y1</f>
         <v/>
       </c>
       <c r="Z20">
-        <f>A18*Z1</f>
+        <f>A15*Z1</f>
         <v/>
       </c>
       <c r="AA20">
-        <f>A18*AA1</f>
+        <f>A15*AA1</f>
         <v/>
       </c>
       <c r="AB20">
-        <f>A18*AB1</f>
+        <f>A15*AB1</f>
         <v/>
       </c>
       <c r="AC20">
-        <f>A18*AC1</f>
+        <f>A15*AC1</f>
         <v/>
       </c>
       <c r="AD20">
@@ -2579,118 +2321,118 @@
     </row>
     <row r="21" spans="1:30">
       <c r="A21" s="1" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B21">
-        <f>A19*B1</f>
+        <f>A16*B1</f>
         <v/>
       </c>
       <c r="C21">
-        <f>A19*C1</f>
+        <f>A16*C1</f>
         <v/>
       </c>
       <c r="D21">
-        <f>A19*D1</f>
+        <f>A16*D1</f>
         <v/>
       </c>
       <c r="E21">
-        <f>A19*E1</f>
+        <f>A16*E1</f>
         <v/>
       </c>
       <c r="F21">
-        <f>A19*F1</f>
+        <f>A16*F1</f>
         <v/>
       </c>
       <c r="G21">
-        <f>A19*G1</f>
+        <f>A16*G1</f>
         <v/>
       </c>
       <c r="H21">
-        <f>A19*H1</f>
+        <f>A16*H1</f>
         <v/>
       </c>
       <c r="I21">
-        <f>A19*I1</f>
+        <f>A16*I1</f>
         <v/>
       </c>
       <c r="J21">
-        <f>A19*J1</f>
+        <f>A16*J1</f>
         <v/>
       </c>
       <c r="K21">
-        <f>A19*K1</f>
+        <f>A16*K1</f>
         <v/>
       </c>
       <c r="L21">
-        <f>A19*L1</f>
+        <f>A16*L1</f>
         <v/>
       </c>
       <c r="M21">
-        <f>A19*M1</f>
+        <f>A16*M1</f>
         <v/>
       </c>
       <c r="N21">
-        <f>A19*N1</f>
+        <f>A16*N1</f>
         <v/>
       </c>
       <c r="O21">
-        <f>A19*O1</f>
+        <f>A16*O1</f>
         <v/>
       </c>
       <c r="P21">
-        <f>A19*P1</f>
+        <f>A16*P1</f>
         <v/>
       </c>
       <c r="Q21">
-        <f>A19*Q1</f>
+        <f>A16*Q1</f>
         <v/>
       </c>
       <c r="R21">
-        <f>A19*R1</f>
+        <f>A16*R1</f>
         <v/>
       </c>
       <c r="S21">
-        <f>A19*S1</f>
+        <f>A16*S1</f>
         <v/>
       </c>
       <c r="T21">
-        <f>A19*T1</f>
+        <f>A16*T1</f>
         <v/>
       </c>
       <c r="U21">
-        <f>A19*U1</f>
+        <f>A16*U1</f>
         <v/>
       </c>
       <c r="V21">
-        <f>A19*V1</f>
+        <f>A16*V1</f>
         <v/>
       </c>
       <c r="W21">
-        <f>A19*W1</f>
+        <f>A16*W1</f>
         <v/>
       </c>
       <c r="X21">
-        <f>A19*X1</f>
+        <f>A16*X1</f>
         <v/>
       </c>
       <c r="Y21">
-        <f>A19*Y1</f>
+        <f>A16*Y1</f>
         <v/>
       </c>
       <c r="Z21">
-        <f>A19*Z1</f>
+        <f>A16*Z1</f>
         <v/>
       </c>
       <c r="AA21">
-        <f>A19*AA1</f>
+        <f>A16*AA1</f>
         <v/>
       </c>
       <c r="AB21">
-        <f>A19*AB1</f>
+        <f>A16*AB1</f>
         <v/>
       </c>
       <c r="AC21">
-        <f>A19*AC1</f>
+        <f>A16*AC1</f>
         <v/>
       </c>
       <c r="AD21">
@@ -2700,118 +2442,118 @@
     </row>
     <row r="22" spans="1:30">
       <c r="A22" s="1" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B22">
-        <f>A20*B1</f>
+        <f>A17*B1</f>
         <v/>
       </c>
       <c r="C22">
-        <f>A20*C1</f>
+        <f>A17*C1</f>
         <v/>
       </c>
       <c r="D22">
-        <f>A20*D1</f>
+        <f>A17*D1</f>
         <v/>
       </c>
       <c r="E22">
-        <f>A20*E1</f>
+        <f>A17*E1</f>
         <v/>
       </c>
       <c r="F22">
-        <f>A20*F1</f>
+        <f>A17*F1</f>
         <v/>
       </c>
       <c r="G22">
-        <f>A20*G1</f>
+        <f>A17*G1</f>
         <v/>
       </c>
       <c r="H22">
-        <f>A20*H1</f>
+        <f>A17*H1</f>
         <v/>
       </c>
       <c r="I22">
-        <f>A20*I1</f>
+        <f>A17*I1</f>
         <v/>
       </c>
       <c r="J22">
-        <f>A20*J1</f>
+        <f>A17*J1</f>
         <v/>
       </c>
       <c r="K22">
-        <f>A20*K1</f>
+        <f>A17*K1</f>
         <v/>
       </c>
       <c r="L22">
-        <f>A20*L1</f>
+        <f>A17*L1</f>
         <v/>
       </c>
       <c r="M22">
-        <f>A20*M1</f>
+        <f>A17*M1</f>
         <v/>
       </c>
       <c r="N22">
-        <f>A20*N1</f>
+        <f>A17*N1</f>
         <v/>
       </c>
       <c r="O22">
-        <f>A20*O1</f>
+        <f>A17*O1</f>
         <v/>
       </c>
       <c r="P22">
-        <f>A20*P1</f>
+        <f>A17*P1</f>
         <v/>
       </c>
       <c r="Q22">
-        <f>A20*Q1</f>
+        <f>A17*Q1</f>
         <v/>
       </c>
       <c r="R22">
-        <f>A20*R1</f>
+        <f>A17*R1</f>
         <v/>
       </c>
       <c r="S22">
-        <f>A20*S1</f>
+        <f>A17*S1</f>
         <v/>
       </c>
       <c r="T22">
-        <f>A20*T1</f>
+        <f>A17*T1</f>
         <v/>
       </c>
       <c r="U22">
-        <f>A20*U1</f>
+        <f>A17*U1</f>
         <v/>
       </c>
       <c r="V22">
-        <f>A20*V1</f>
+        <f>A17*V1</f>
         <v/>
       </c>
       <c r="W22">
-        <f>A20*W1</f>
+        <f>A17*W1</f>
         <v/>
       </c>
       <c r="X22">
-        <f>A20*X1</f>
+        <f>A17*X1</f>
         <v/>
       </c>
       <c r="Y22">
-        <f>A20*Y1</f>
+        <f>A17*Y1</f>
         <v/>
       </c>
       <c r="Z22">
-        <f>A20*Z1</f>
+        <f>A17*Z1</f>
         <v/>
       </c>
       <c r="AA22">
-        <f>A20*AA1</f>
+        <f>A17*AA1</f>
         <v/>
       </c>
       <c r="AB22">
-        <f>A20*AB1</f>
+        <f>A17*AB1</f>
         <v/>
       </c>
       <c r="AC22">
-        <f>A20*AC1</f>
+        <f>A17*AC1</f>
         <v/>
       </c>
       <c r="AD22">
@@ -2821,118 +2563,118 @@
     </row>
     <row r="23" spans="1:30">
       <c r="A23" s="1" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B23">
-        <f>A21*B1</f>
+        <f>A18*B1</f>
         <v/>
       </c>
       <c r="C23">
-        <f>A21*C1</f>
+        <f>A18*C1</f>
         <v/>
       </c>
       <c r="D23">
-        <f>A21*D1</f>
+        <f>A18*D1</f>
         <v/>
       </c>
       <c r="E23">
-        <f>A21*E1</f>
+        <f>A18*E1</f>
         <v/>
       </c>
       <c r="F23">
-        <f>A21*F1</f>
+        <f>A18*F1</f>
         <v/>
       </c>
       <c r="G23">
-        <f>A21*G1</f>
+        <f>A18*G1</f>
         <v/>
       </c>
       <c r="H23">
-        <f>A21*H1</f>
+        <f>A18*H1</f>
         <v/>
       </c>
       <c r="I23">
-        <f>A21*I1</f>
+        <f>A18*I1</f>
         <v/>
       </c>
       <c r="J23">
-        <f>A21*J1</f>
+        <f>A18*J1</f>
         <v/>
       </c>
       <c r="K23">
-        <f>A21*K1</f>
+        <f>A18*K1</f>
         <v/>
       </c>
       <c r="L23">
-        <f>A21*L1</f>
+        <f>A18*L1</f>
         <v/>
       </c>
       <c r="M23">
-        <f>A21*M1</f>
+        <f>A18*M1</f>
         <v/>
       </c>
       <c r="N23">
-        <f>A21*N1</f>
+        <f>A18*N1</f>
         <v/>
       </c>
       <c r="O23">
-        <f>A21*O1</f>
+        <f>A18*O1</f>
         <v/>
       </c>
       <c r="P23">
-        <f>A21*P1</f>
+        <f>A18*P1</f>
         <v/>
       </c>
       <c r="Q23">
-        <f>A21*Q1</f>
+        <f>A18*Q1</f>
         <v/>
       </c>
       <c r="R23">
-        <f>A21*R1</f>
+        <f>A18*R1</f>
         <v/>
       </c>
       <c r="S23">
-        <f>A21*S1</f>
+        <f>A18*S1</f>
         <v/>
       </c>
       <c r="T23">
-        <f>A21*T1</f>
+        <f>A18*T1</f>
         <v/>
       </c>
       <c r="U23">
-        <f>A21*U1</f>
+        <f>A18*U1</f>
         <v/>
       </c>
       <c r="V23">
-        <f>A21*V1</f>
+        <f>A18*V1</f>
         <v/>
       </c>
       <c r="W23">
-        <f>A21*W1</f>
+        <f>A18*W1</f>
         <v/>
       </c>
       <c r="X23">
-        <f>A21*X1</f>
+        <f>A18*X1</f>
         <v/>
       </c>
       <c r="Y23">
-        <f>A21*Y1</f>
+        <f>A18*Y1</f>
         <v/>
       </c>
       <c r="Z23">
-        <f>A21*Z1</f>
+        <f>A18*Z1</f>
         <v/>
       </c>
       <c r="AA23">
-        <f>A21*AA1</f>
+        <f>A18*AA1</f>
         <v/>
       </c>
       <c r="AB23">
-        <f>A21*AB1</f>
+        <f>A18*AB1</f>
         <v/>
       </c>
       <c r="AC23">
-        <f>A21*AC1</f>
+        <f>A18*AC1</f>
         <v/>
       </c>
       <c r="AD23">
@@ -2942,118 +2684,118 @@
     </row>
     <row r="24" spans="1:30">
       <c r="A24" s="1" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B24">
-        <f>A22*B1</f>
+        <f>A19*B1</f>
         <v/>
       </c>
       <c r="C24">
-        <f>A22*C1</f>
+        <f>A19*C1</f>
         <v/>
       </c>
       <c r="D24">
-        <f>A22*D1</f>
+        <f>A19*D1</f>
         <v/>
       </c>
       <c r="E24">
-        <f>A22*E1</f>
+        <f>A19*E1</f>
         <v/>
       </c>
       <c r="F24">
-        <f>A22*F1</f>
+        <f>A19*F1</f>
         <v/>
       </c>
       <c r="G24">
-        <f>A22*G1</f>
+        <f>A19*G1</f>
         <v/>
       </c>
       <c r="H24">
-        <f>A22*H1</f>
+        <f>A19*H1</f>
         <v/>
       </c>
       <c r="I24">
-        <f>A22*I1</f>
+        <f>A19*I1</f>
         <v/>
       </c>
       <c r="J24">
-        <f>A22*J1</f>
+        <f>A19*J1</f>
         <v/>
       </c>
       <c r="K24">
-        <f>A22*K1</f>
+        <f>A19*K1</f>
         <v/>
       </c>
       <c r="L24">
-        <f>A22*L1</f>
+        <f>A19*L1</f>
         <v/>
       </c>
       <c r="M24">
-        <f>A22*M1</f>
+        <f>A19*M1</f>
         <v/>
       </c>
       <c r="N24">
-        <f>A22*N1</f>
+        <f>A19*N1</f>
         <v/>
       </c>
       <c r="O24">
-        <f>A22*O1</f>
+        <f>A19*O1</f>
         <v/>
       </c>
       <c r="P24">
-        <f>A22*P1</f>
+        <f>A19*P1</f>
         <v/>
       </c>
       <c r="Q24">
-        <f>A22*Q1</f>
+        <f>A19*Q1</f>
         <v/>
       </c>
       <c r="R24">
-        <f>A22*R1</f>
+        <f>A19*R1</f>
         <v/>
       </c>
       <c r="S24">
-        <f>A22*S1</f>
+        <f>A19*S1</f>
         <v/>
       </c>
       <c r="T24">
-        <f>A22*T1</f>
+        <f>A19*T1</f>
         <v/>
       </c>
       <c r="U24">
-        <f>A22*U1</f>
+        <f>A19*U1</f>
         <v/>
       </c>
       <c r="V24">
-        <f>A22*V1</f>
+        <f>A19*V1</f>
         <v/>
       </c>
       <c r="W24">
-        <f>A22*W1</f>
+        <f>A19*W1</f>
         <v/>
       </c>
       <c r="X24">
-        <f>A22*X1</f>
+        <f>A19*X1</f>
         <v/>
       </c>
       <c r="Y24">
-        <f>A22*Y1</f>
+        <f>A19*Y1</f>
         <v/>
       </c>
       <c r="Z24">
-        <f>A22*Z1</f>
+        <f>A19*Z1</f>
         <v/>
       </c>
       <c r="AA24">
-        <f>A22*AA1</f>
+        <f>A19*AA1</f>
         <v/>
       </c>
       <c r="AB24">
-        <f>A22*AB1</f>
+        <f>A19*AB1</f>
         <v/>
       </c>
       <c r="AC24">
-        <f>A22*AC1</f>
+        <f>A19*AC1</f>
         <v/>
       </c>
       <c r="AD24">
@@ -3063,118 +2805,118 @@
     </row>
     <row r="25" spans="1:30">
       <c r="A25" s="1" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B25">
-        <f>A23*B1</f>
+        <f>A20*B1</f>
         <v/>
       </c>
       <c r="C25">
-        <f>A23*C1</f>
+        <f>A20*C1</f>
         <v/>
       </c>
       <c r="D25">
-        <f>A23*D1</f>
+        <f>A20*D1</f>
         <v/>
       </c>
       <c r="E25">
-        <f>A23*E1</f>
+        <f>A20*E1</f>
         <v/>
       </c>
       <c r="F25">
-        <f>A23*F1</f>
+        <f>A20*F1</f>
         <v/>
       </c>
       <c r="G25">
-        <f>A23*G1</f>
+        <f>A20*G1</f>
         <v/>
       </c>
       <c r="H25">
-        <f>A23*H1</f>
+        <f>A20*H1</f>
         <v/>
       </c>
       <c r="I25">
-        <f>A23*I1</f>
+        <f>A20*I1</f>
         <v/>
       </c>
       <c r="J25">
-        <f>A23*J1</f>
+        <f>A20*J1</f>
         <v/>
       </c>
       <c r="K25">
-        <f>A23*K1</f>
+        <f>A20*K1</f>
         <v/>
       </c>
       <c r="L25">
-        <f>A23*L1</f>
+        <f>A20*L1</f>
         <v/>
       </c>
       <c r="M25">
-        <f>A23*M1</f>
+        <f>A20*M1</f>
         <v/>
       </c>
       <c r="N25">
-        <f>A23*N1</f>
+        <f>A20*N1</f>
         <v/>
       </c>
       <c r="O25">
-        <f>A23*O1</f>
+        <f>A20*O1</f>
         <v/>
       </c>
       <c r="P25">
-        <f>A23*P1</f>
+        <f>A20*P1</f>
         <v/>
       </c>
       <c r="Q25">
-        <f>A23*Q1</f>
+        <f>A20*Q1</f>
         <v/>
       </c>
       <c r="R25">
-        <f>A23*R1</f>
+        <f>A20*R1</f>
         <v/>
       </c>
       <c r="S25">
-        <f>A23*S1</f>
+        <f>A20*S1</f>
         <v/>
       </c>
       <c r="T25">
-        <f>A23*T1</f>
+        <f>A20*T1</f>
         <v/>
       </c>
       <c r="U25">
-        <f>A23*U1</f>
+        <f>A20*U1</f>
         <v/>
       </c>
       <c r="V25">
-        <f>A23*V1</f>
+        <f>A20*V1</f>
         <v/>
       </c>
       <c r="W25">
-        <f>A23*W1</f>
+        <f>A20*W1</f>
         <v/>
       </c>
       <c r="X25">
-        <f>A23*X1</f>
+        <f>A20*X1</f>
         <v/>
       </c>
       <c r="Y25">
-        <f>A23*Y1</f>
+        <f>A20*Y1</f>
         <v/>
       </c>
       <c r="Z25">
-        <f>A23*Z1</f>
+        <f>A20*Z1</f>
         <v/>
       </c>
       <c r="AA25">
-        <f>A23*AA1</f>
+        <f>A20*AA1</f>
         <v/>
       </c>
       <c r="AB25">
-        <f>A23*AB1</f>
+        <f>A20*AB1</f>
         <v/>
       </c>
       <c r="AC25">
-        <f>A23*AC1</f>
+        <f>A20*AC1</f>
         <v/>
       </c>
       <c r="AD25">
@@ -3184,118 +2926,118 @@
     </row>
     <row r="26" spans="1:30">
       <c r="A26" s="1" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B26">
-        <f>A24*B1</f>
+        <f>A21*B1</f>
         <v/>
       </c>
       <c r="C26">
-        <f>A24*C1</f>
+        <f>A21*C1</f>
         <v/>
       </c>
       <c r="D26">
-        <f>A24*D1</f>
+        <f>A21*D1</f>
         <v/>
       </c>
       <c r="E26">
-        <f>A24*E1</f>
+        <f>A21*E1</f>
         <v/>
       </c>
       <c r="F26">
-        <f>A24*F1</f>
+        <f>A21*F1</f>
         <v/>
       </c>
       <c r="G26">
-        <f>A24*G1</f>
+        <f>A21*G1</f>
         <v/>
       </c>
       <c r="H26">
-        <f>A24*H1</f>
+        <f>A21*H1</f>
         <v/>
       </c>
       <c r="I26">
-        <f>A24*I1</f>
+        <f>A21*I1</f>
         <v/>
       </c>
       <c r="J26">
-        <f>A24*J1</f>
+        <f>A21*J1</f>
         <v/>
       </c>
       <c r="K26">
-        <f>A24*K1</f>
+        <f>A21*K1</f>
         <v/>
       </c>
       <c r="L26">
-        <f>A24*L1</f>
+        <f>A21*L1</f>
         <v/>
       </c>
       <c r="M26">
-        <f>A24*M1</f>
+        <f>A21*M1</f>
         <v/>
       </c>
       <c r="N26">
-        <f>A24*N1</f>
+        <f>A21*N1</f>
         <v/>
       </c>
       <c r="O26">
-        <f>A24*O1</f>
+        <f>A21*O1</f>
         <v/>
       </c>
       <c r="P26">
-        <f>A24*P1</f>
+        <f>A21*P1</f>
         <v/>
       </c>
       <c r="Q26">
-        <f>A24*Q1</f>
+        <f>A21*Q1</f>
         <v/>
       </c>
       <c r="R26">
-        <f>A24*R1</f>
+        <f>A21*R1</f>
         <v/>
       </c>
       <c r="S26">
-        <f>A24*S1</f>
+        <f>A21*S1</f>
         <v/>
       </c>
       <c r="T26">
-        <f>A24*T1</f>
+        <f>A21*T1</f>
         <v/>
       </c>
       <c r="U26">
-        <f>A24*U1</f>
+        <f>A21*U1</f>
         <v/>
       </c>
       <c r="V26">
-        <f>A24*V1</f>
+        <f>A21*V1</f>
         <v/>
       </c>
       <c r="W26">
-        <f>A24*W1</f>
+        <f>A21*W1</f>
         <v/>
       </c>
       <c r="X26">
-        <f>A24*X1</f>
+        <f>A21*X1</f>
         <v/>
       </c>
       <c r="Y26">
-        <f>A24*Y1</f>
+        <f>A21*Y1</f>
         <v/>
       </c>
       <c r="Z26">
-        <f>A24*Z1</f>
+        <f>A21*Z1</f>
         <v/>
       </c>
       <c r="AA26">
-        <f>A24*AA1</f>
+        <f>A21*AA1</f>
         <v/>
       </c>
       <c r="AB26">
-        <f>A24*AB1</f>
+        <f>A21*AB1</f>
         <v/>
       </c>
       <c r="AC26">
-        <f>A24*AC1</f>
+        <f>A21*AC1</f>
         <v/>
       </c>
       <c r="AD26">
@@ -3305,118 +3047,118 @@
     </row>
     <row r="27" spans="1:30">
       <c r="A27" s="1" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B27">
-        <f>A25*B1</f>
+        <f>A22*B1</f>
         <v/>
       </c>
       <c r="C27">
-        <f>A25*C1</f>
+        <f>A22*C1</f>
         <v/>
       </c>
       <c r="D27">
-        <f>A25*D1</f>
+        <f>A22*D1</f>
         <v/>
       </c>
       <c r="E27">
-        <f>A25*E1</f>
+        <f>A22*E1</f>
         <v/>
       </c>
       <c r="F27">
-        <f>A25*F1</f>
+        <f>A22*F1</f>
         <v/>
       </c>
       <c r="G27">
-        <f>A25*G1</f>
+        <f>A22*G1</f>
         <v/>
       </c>
       <c r="H27">
-        <f>A25*H1</f>
+        <f>A22*H1</f>
         <v/>
       </c>
       <c r="I27">
-        <f>A25*I1</f>
+        <f>A22*I1</f>
         <v/>
       </c>
       <c r="J27">
-        <f>A25*J1</f>
+        <f>A22*J1</f>
         <v/>
       </c>
       <c r="K27">
-        <f>A25*K1</f>
+        <f>A22*K1</f>
         <v/>
       </c>
       <c r="L27">
-        <f>A25*L1</f>
+        <f>A22*L1</f>
         <v/>
       </c>
       <c r="M27">
-        <f>A25*M1</f>
+        <f>A22*M1</f>
         <v/>
       </c>
       <c r="N27">
-        <f>A25*N1</f>
+        <f>A22*N1</f>
         <v/>
       </c>
       <c r="O27">
-        <f>A25*O1</f>
+        <f>A22*O1</f>
         <v/>
       </c>
       <c r="P27">
-        <f>A25*P1</f>
+        <f>A22*P1</f>
         <v/>
       </c>
       <c r="Q27">
-        <f>A25*Q1</f>
+        <f>A22*Q1</f>
         <v/>
       </c>
       <c r="R27">
-        <f>A25*R1</f>
+        <f>A22*R1</f>
         <v/>
       </c>
       <c r="S27">
-        <f>A25*S1</f>
+        <f>A22*S1</f>
         <v/>
       </c>
       <c r="T27">
-        <f>A25*T1</f>
+        <f>A22*T1</f>
         <v/>
       </c>
       <c r="U27">
-        <f>A25*U1</f>
+        <f>A22*U1</f>
         <v/>
       </c>
       <c r="V27">
-        <f>A25*V1</f>
+        <f>A22*V1</f>
         <v/>
       </c>
       <c r="W27">
-        <f>A25*W1</f>
+        <f>A22*W1</f>
         <v/>
       </c>
       <c r="X27">
-        <f>A25*X1</f>
+        <f>A22*X1</f>
         <v/>
       </c>
       <c r="Y27">
-        <f>A25*Y1</f>
+        <f>A22*Y1</f>
         <v/>
       </c>
       <c r="Z27">
-        <f>A25*Z1</f>
+        <f>A22*Z1</f>
         <v/>
       </c>
       <c r="AA27">
-        <f>A25*AA1</f>
+        <f>A22*AA1</f>
         <v/>
       </c>
       <c r="AB27">
-        <f>A25*AB1</f>
+        <f>A22*AB1</f>
         <v/>
       </c>
       <c r="AC27">
-        <f>A25*AC1</f>
+        <f>A22*AC1</f>
         <v/>
       </c>
       <c r="AD27">
@@ -3426,118 +3168,118 @@
     </row>
     <row r="28" spans="1:30">
       <c r="A28" s="1" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B28">
-        <f>A26*B1</f>
+        <f>A23*B1</f>
         <v/>
       </c>
       <c r="C28">
-        <f>A26*C1</f>
+        <f>A23*C1</f>
         <v/>
       </c>
       <c r="D28">
-        <f>A26*D1</f>
+        <f>A23*D1</f>
         <v/>
       </c>
       <c r="E28">
-        <f>A26*E1</f>
+        <f>A23*E1</f>
         <v/>
       </c>
       <c r="F28">
-        <f>A26*F1</f>
+        <f>A23*F1</f>
         <v/>
       </c>
       <c r="G28">
-        <f>A26*G1</f>
+        <f>A23*G1</f>
         <v/>
       </c>
       <c r="H28">
-        <f>A26*H1</f>
+        <f>A23*H1</f>
         <v/>
       </c>
       <c r="I28">
-        <f>A26*I1</f>
+        <f>A23*I1</f>
         <v/>
       </c>
       <c r="J28">
-        <f>A26*J1</f>
+        <f>A23*J1</f>
         <v/>
       </c>
       <c r="K28">
-        <f>A26*K1</f>
+        <f>A23*K1</f>
         <v/>
       </c>
       <c r="L28">
-        <f>A26*L1</f>
+        <f>A23*L1</f>
         <v/>
       </c>
       <c r="M28">
-        <f>A26*M1</f>
+        <f>A23*M1</f>
         <v/>
       </c>
       <c r="N28">
-        <f>A26*N1</f>
+        <f>A23*N1</f>
         <v/>
       </c>
       <c r="O28">
-        <f>A26*O1</f>
+        <f>A23*O1</f>
         <v/>
       </c>
       <c r="P28">
-        <f>A26*P1</f>
+        <f>A23*P1</f>
         <v/>
       </c>
       <c r="Q28">
-        <f>A26*Q1</f>
+        <f>A23*Q1</f>
         <v/>
       </c>
       <c r="R28">
-        <f>A26*R1</f>
+        <f>A23*R1</f>
         <v/>
       </c>
       <c r="S28">
-        <f>A26*S1</f>
+        <f>A23*S1</f>
         <v/>
       </c>
       <c r="T28">
-        <f>A26*T1</f>
+        <f>A23*T1</f>
         <v/>
       </c>
       <c r="U28">
-        <f>A26*U1</f>
+        <f>A23*U1</f>
         <v/>
       </c>
       <c r="V28">
-        <f>A26*V1</f>
+        <f>A23*V1</f>
         <v/>
       </c>
       <c r="W28">
-        <f>A26*W1</f>
+        <f>A23*W1</f>
         <v/>
       </c>
       <c r="X28">
-        <f>A26*X1</f>
+        <f>A23*X1</f>
         <v/>
       </c>
       <c r="Y28">
-        <f>A26*Y1</f>
+        <f>A23*Y1</f>
         <v/>
       </c>
       <c r="Z28">
-        <f>A26*Z1</f>
+        <f>A23*Z1</f>
         <v/>
       </c>
       <c r="AA28">
-        <f>A26*AA1</f>
+        <f>A23*AA1</f>
         <v/>
       </c>
       <c r="AB28">
-        <f>A26*AB1</f>
+        <f>A23*AB1</f>
         <v/>
       </c>
       <c r="AC28">
-        <f>A26*AC1</f>
+        <f>A23*AC1</f>
         <v/>
       </c>
       <c r="AD28">
@@ -3547,118 +3289,118 @@
     </row>
     <row r="29" spans="1:30">
       <c r="A29" s="1" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B29">
-        <f>A27*B1</f>
+        <f>A24*B1</f>
         <v/>
       </c>
       <c r="C29">
-        <f>A27*C1</f>
+        <f>A24*C1</f>
         <v/>
       </c>
       <c r="D29">
-        <f>A27*D1</f>
+        <f>A24*D1</f>
         <v/>
       </c>
       <c r="E29">
-        <f>A27*E1</f>
+        <f>A24*E1</f>
         <v/>
       </c>
       <c r="F29">
-        <f>A27*F1</f>
+        <f>A24*F1</f>
         <v/>
       </c>
       <c r="G29">
-        <f>A27*G1</f>
+        <f>A24*G1</f>
         <v/>
       </c>
       <c r="H29">
-        <f>A27*H1</f>
+        <f>A24*H1</f>
         <v/>
       </c>
       <c r="I29">
-        <f>A27*I1</f>
+        <f>A24*I1</f>
         <v/>
       </c>
       <c r="J29">
-        <f>A27*J1</f>
+        <f>A24*J1</f>
         <v/>
       </c>
       <c r="K29">
-        <f>A27*K1</f>
+        <f>A24*K1</f>
         <v/>
       </c>
       <c r="L29">
-        <f>A27*L1</f>
+        <f>A24*L1</f>
         <v/>
       </c>
       <c r="M29">
-        <f>A27*M1</f>
+        <f>A24*M1</f>
         <v/>
       </c>
       <c r="N29">
-        <f>A27*N1</f>
+        <f>A24*N1</f>
         <v/>
       </c>
       <c r="O29">
-        <f>A27*O1</f>
+        <f>A24*O1</f>
         <v/>
       </c>
       <c r="P29">
-        <f>A27*P1</f>
+        <f>A24*P1</f>
         <v/>
       </c>
       <c r="Q29">
-        <f>A27*Q1</f>
+        <f>A24*Q1</f>
         <v/>
       </c>
       <c r="R29">
-        <f>A27*R1</f>
+        <f>A24*R1</f>
         <v/>
       </c>
       <c r="S29">
-        <f>A27*S1</f>
+        <f>A24*S1</f>
         <v/>
       </c>
       <c r="T29">
-        <f>A27*T1</f>
+        <f>A24*T1</f>
         <v/>
       </c>
       <c r="U29">
-        <f>A27*U1</f>
+        <f>A24*U1</f>
         <v/>
       </c>
       <c r="V29">
-        <f>A27*V1</f>
+        <f>A24*V1</f>
         <v/>
       </c>
       <c r="W29">
-        <f>A27*W1</f>
+        <f>A24*W1</f>
         <v/>
       </c>
       <c r="X29">
-        <f>A27*X1</f>
+        <f>A24*X1</f>
         <v/>
       </c>
       <c r="Y29">
-        <f>A27*Y1</f>
+        <f>A24*Y1</f>
         <v/>
       </c>
       <c r="Z29">
-        <f>A27*Z1</f>
+        <f>A24*Z1</f>
         <v/>
       </c>
       <c r="AA29">
-        <f>A27*AA1</f>
+        <f>A24*AA1</f>
         <v/>
       </c>
       <c r="AB29">
-        <f>A27*AB1</f>
+        <f>A24*AB1</f>
         <v/>
       </c>
       <c r="AC29">
-        <f>A27*AC1</f>
+        <f>A24*AC1</f>
         <v/>
       </c>
       <c r="AD29">
@@ -3668,118 +3410,118 @@
     </row>
     <row r="30" spans="1:30">
       <c r="A30" s="1" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B30">
-        <f>A28*B1</f>
+        <f>A25*B1</f>
         <v/>
       </c>
       <c r="C30">
-        <f>A28*C1</f>
+        <f>A25*C1</f>
         <v/>
       </c>
       <c r="D30">
-        <f>A28*D1</f>
+        <f>A25*D1</f>
         <v/>
       </c>
       <c r="E30">
-        <f>A28*E1</f>
+        <f>A25*E1</f>
         <v/>
       </c>
       <c r="F30">
-        <f>A28*F1</f>
+        <f>A25*F1</f>
         <v/>
       </c>
       <c r="G30">
-        <f>A28*G1</f>
+        <f>A25*G1</f>
         <v/>
       </c>
       <c r="H30">
-        <f>A28*H1</f>
+        <f>A25*H1</f>
         <v/>
       </c>
       <c r="I30">
-        <f>A28*I1</f>
+        <f>A25*I1</f>
         <v/>
       </c>
       <c r="J30">
-        <f>A28*J1</f>
+        <f>A25*J1</f>
         <v/>
       </c>
       <c r="K30">
-        <f>A28*K1</f>
+        <f>A25*K1</f>
         <v/>
       </c>
       <c r="L30">
-        <f>A28*L1</f>
+        <f>A25*L1</f>
         <v/>
       </c>
       <c r="M30">
-        <f>A28*M1</f>
+        <f>A25*M1</f>
         <v/>
       </c>
       <c r="N30">
-        <f>A28*N1</f>
+        <f>A25*N1</f>
         <v/>
       </c>
       <c r="O30">
-        <f>A28*O1</f>
+        <f>A25*O1</f>
         <v/>
       </c>
       <c r="P30">
-        <f>A28*P1</f>
+        <f>A25*P1</f>
         <v/>
       </c>
       <c r="Q30">
-        <f>A28*Q1</f>
+        <f>A25*Q1</f>
         <v/>
       </c>
       <c r="R30">
-        <f>A28*R1</f>
+        <f>A25*R1</f>
         <v/>
       </c>
       <c r="S30">
-        <f>A28*S1</f>
+        <f>A25*S1</f>
         <v/>
       </c>
       <c r="T30">
-        <f>A28*T1</f>
+        <f>A25*T1</f>
         <v/>
       </c>
       <c r="U30">
-        <f>A28*U1</f>
+        <f>A25*U1</f>
         <v/>
       </c>
       <c r="V30">
-        <f>A28*V1</f>
+        <f>A25*V1</f>
         <v/>
       </c>
       <c r="W30">
-        <f>A28*W1</f>
+        <f>A25*W1</f>
         <v/>
       </c>
       <c r="X30">
-        <f>A28*X1</f>
+        <f>A25*X1</f>
         <v/>
       </c>
       <c r="Y30">
-        <f>A28*Y1</f>
+        <f>A25*Y1</f>
         <v/>
       </c>
       <c r="Z30">
-        <f>A28*Z1</f>
+        <f>A25*Z1</f>
         <v/>
       </c>
       <c r="AA30">
-        <f>A28*AA1</f>
+        <f>A25*AA1</f>
         <v/>
       </c>
       <c r="AB30">
-        <f>A28*AB1</f>
+        <f>A25*AB1</f>
         <v/>
       </c>
       <c r="AC30">
-        <f>A28*AC1</f>
+        <f>A25*AC1</f>
         <v/>
       </c>
       <c r="AD30">
@@ -3789,234 +3531,585 @@
     </row>
     <row r="31" spans="1:30">
       <c r="A31" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B31">
-        <f>A29*B1</f>
+        <f>A26*B1</f>
         <v/>
       </c>
       <c r="C31">
-        <f>A29*C1</f>
+        <f>A26*C1</f>
         <v/>
       </c>
       <c r="D31">
-        <f>A29*D1</f>
+        <f>A26*D1</f>
         <v/>
       </c>
       <c r="E31">
-        <f>A29*E1</f>
+        <f>A26*E1</f>
         <v/>
       </c>
       <c r="F31">
-        <f>A29*F1</f>
+        <f>A26*F1</f>
         <v/>
       </c>
       <c r="G31">
-        <f>A29*G1</f>
+        <f>A26*G1</f>
         <v/>
       </c>
       <c r="H31">
-        <f>A29*H1</f>
+        <f>A26*H1</f>
         <v/>
       </c>
       <c r="I31">
-        <f>A29*I1</f>
+        <f>A26*I1</f>
         <v/>
       </c>
       <c r="J31">
-        <f>A29*J1</f>
+        <f>A26*J1</f>
         <v/>
       </c>
       <c r="K31">
-        <f>A29*K1</f>
+        <f>A26*K1</f>
         <v/>
       </c>
       <c r="L31">
-        <f>A29*L1</f>
+        <f>A26*L1</f>
         <v/>
       </c>
       <c r="M31">
-        <f>A29*M1</f>
+        <f>A26*M1</f>
         <v/>
       </c>
       <c r="N31">
-        <f>A29*N1</f>
+        <f>A26*N1</f>
         <v/>
       </c>
       <c r="O31">
-        <f>A29*O1</f>
+        <f>A26*O1</f>
         <v/>
       </c>
       <c r="P31">
-        <f>A29*P1</f>
+        <f>A26*P1</f>
         <v/>
       </c>
       <c r="Q31">
-        <f>A29*Q1</f>
+        <f>A26*Q1</f>
         <v/>
       </c>
       <c r="R31">
-        <f>A29*R1</f>
+        <f>A26*R1</f>
         <v/>
       </c>
       <c r="S31">
-        <f>A29*S1</f>
+        <f>A26*S1</f>
         <v/>
       </c>
       <c r="T31">
-        <f>A29*T1</f>
+        <f>A26*T1</f>
         <v/>
       </c>
       <c r="U31">
-        <f>A29*U1</f>
+        <f>A26*U1</f>
         <v/>
       </c>
       <c r="V31">
-        <f>A29*V1</f>
+        <f>A26*V1</f>
         <v/>
       </c>
       <c r="W31">
-        <f>A29*W1</f>
+        <f>A26*W1</f>
         <v/>
       </c>
       <c r="X31">
-        <f>A29*X1</f>
+        <f>A26*X1</f>
         <v/>
       </c>
       <c r="Y31">
-        <f>A29*Y1</f>
+        <f>A26*Y1</f>
         <v/>
       </c>
       <c r="Z31">
-        <f>A29*Z1</f>
+        <f>A26*Z1</f>
         <v/>
       </c>
       <c r="AA31">
-        <f>A29*AA1</f>
+        <f>A26*AA1</f>
         <v/>
       </c>
       <c r="AB31">
-        <f>A29*AB1</f>
+        <f>A26*AB1</f>
         <v/>
       </c>
       <c r="AC31">
-        <f>A29*AC1</f>
+        <f>A26*AC1</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:30">
       <c r="A32" t="n">
+        <v>26</v>
+      </c>
+      <c r="B32">
+        <f>A27*B1</f>
+        <v/>
+      </c>
+      <c r="C32">
+        <f>A27*C1</f>
+        <v/>
+      </c>
+      <c r="D32">
+        <f>A27*D1</f>
+        <v/>
+      </c>
+      <c r="E32">
+        <f>A27*E1</f>
+        <v/>
+      </c>
+      <c r="F32">
+        <f>A27*F1</f>
+        <v/>
+      </c>
+      <c r="G32">
+        <f>A27*G1</f>
+        <v/>
+      </c>
+      <c r="H32">
+        <f>A27*H1</f>
+        <v/>
+      </c>
+      <c r="I32">
+        <f>A27*I1</f>
+        <v/>
+      </c>
+      <c r="J32">
+        <f>A27*J1</f>
+        <v/>
+      </c>
+      <c r="K32">
+        <f>A27*K1</f>
+        <v/>
+      </c>
+      <c r="L32">
+        <f>A27*L1</f>
+        <v/>
+      </c>
+      <c r="M32">
+        <f>A27*M1</f>
+        <v/>
+      </c>
+      <c r="N32">
+        <f>A27*N1</f>
+        <v/>
+      </c>
+      <c r="O32">
+        <f>A27*O1</f>
+        <v/>
+      </c>
+      <c r="P32">
+        <f>A27*P1</f>
+        <v/>
+      </c>
+      <c r="Q32">
+        <f>A27*Q1</f>
+        <v/>
+      </c>
+      <c r="R32">
+        <f>A27*R1</f>
+        <v/>
+      </c>
+      <c r="S32">
+        <f>A27*S1</f>
+        <v/>
+      </c>
+      <c r="T32">
+        <f>A27*T1</f>
+        <v/>
+      </c>
+      <c r="U32">
+        <f>A27*U1</f>
+        <v/>
+      </c>
+      <c r="V32">
+        <f>A27*V1</f>
+        <v/>
+      </c>
+      <c r="W32">
+        <f>A27*W1</f>
+        <v/>
+      </c>
+      <c r="X32">
+        <f>A27*X1</f>
+        <v/>
+      </c>
+      <c r="Y32">
+        <f>A27*Y1</f>
+        <v/>
+      </c>
+      <c r="Z32">
+        <f>A27*Z1</f>
+        <v/>
+      </c>
+      <c r="AA32">
+        <f>A27*AA1</f>
+        <v/>
+      </c>
+      <c r="AB32">
+        <f>A27*AB1</f>
+        <v/>
+      </c>
+      <c r="AC32">
+        <f>A27*AC1</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:30">
+      <c r="A33" t="n">
+        <v>27</v>
+      </c>
+      <c r="B33">
+        <f>A28*B1</f>
+        <v/>
+      </c>
+      <c r="C33">
+        <f>A28*C1</f>
+        <v/>
+      </c>
+      <c r="D33">
+        <f>A28*D1</f>
+        <v/>
+      </c>
+      <c r="E33">
+        <f>A28*E1</f>
+        <v/>
+      </c>
+      <c r="F33">
+        <f>A28*F1</f>
+        <v/>
+      </c>
+      <c r="G33">
+        <f>A28*G1</f>
+        <v/>
+      </c>
+      <c r="H33">
+        <f>A28*H1</f>
+        <v/>
+      </c>
+      <c r="I33">
+        <f>A28*I1</f>
+        <v/>
+      </c>
+      <c r="J33">
+        <f>A28*J1</f>
+        <v/>
+      </c>
+      <c r="K33">
+        <f>A28*K1</f>
+        <v/>
+      </c>
+      <c r="L33">
+        <f>A28*L1</f>
+        <v/>
+      </c>
+      <c r="M33">
+        <f>A28*M1</f>
+        <v/>
+      </c>
+      <c r="N33">
+        <f>A28*N1</f>
+        <v/>
+      </c>
+      <c r="O33">
+        <f>A28*O1</f>
+        <v/>
+      </c>
+      <c r="P33">
+        <f>A28*P1</f>
+        <v/>
+      </c>
+      <c r="Q33">
+        <f>A28*Q1</f>
+        <v/>
+      </c>
+      <c r="R33">
+        <f>A28*R1</f>
+        <v/>
+      </c>
+      <c r="S33">
+        <f>A28*S1</f>
+        <v/>
+      </c>
+      <c r="T33">
+        <f>A28*T1</f>
+        <v/>
+      </c>
+      <c r="U33">
+        <f>A28*U1</f>
+        <v/>
+      </c>
+      <c r="V33">
+        <f>A28*V1</f>
+        <v/>
+      </c>
+      <c r="W33">
+        <f>A28*W1</f>
+        <v/>
+      </c>
+      <c r="X33">
+        <f>A28*X1</f>
+        <v/>
+      </c>
+      <c r="Y33">
+        <f>A28*Y1</f>
+        <v/>
+      </c>
+      <c r="Z33">
+        <f>A28*Z1</f>
+        <v/>
+      </c>
+      <c r="AA33">
+        <f>A28*AA1</f>
+        <v/>
+      </c>
+      <c r="AB33">
+        <f>A28*AB1</f>
+        <v/>
+      </c>
+      <c r="AC33">
+        <f>A28*AC1</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:30">
+      <c r="A34" t="n">
+        <v>28</v>
+      </c>
+      <c r="B34">
+        <f>A29*B1</f>
+        <v/>
+      </c>
+      <c r="C34">
+        <f>A29*C1</f>
+        <v/>
+      </c>
+      <c r="D34">
+        <f>A29*D1</f>
+        <v/>
+      </c>
+      <c r="E34">
+        <f>A29*E1</f>
+        <v/>
+      </c>
+      <c r="F34">
+        <f>A29*F1</f>
+        <v/>
+      </c>
+      <c r="G34">
+        <f>A29*G1</f>
+        <v/>
+      </c>
+      <c r="H34">
+        <f>A29*H1</f>
+        <v/>
+      </c>
+      <c r="I34">
+        <f>A29*I1</f>
+        <v/>
+      </c>
+      <c r="J34">
+        <f>A29*J1</f>
+        <v/>
+      </c>
+      <c r="K34">
+        <f>A29*K1</f>
+        <v/>
+      </c>
+      <c r="L34">
+        <f>A29*L1</f>
+        <v/>
+      </c>
+      <c r="M34">
+        <f>A29*M1</f>
+        <v/>
+      </c>
+      <c r="N34">
+        <f>A29*N1</f>
+        <v/>
+      </c>
+      <c r="O34">
+        <f>A29*O1</f>
+        <v/>
+      </c>
+      <c r="P34">
+        <f>A29*P1</f>
+        <v/>
+      </c>
+      <c r="Q34">
+        <f>A29*Q1</f>
+        <v/>
+      </c>
+      <c r="R34">
+        <f>A29*R1</f>
+        <v/>
+      </c>
+      <c r="S34">
+        <f>A29*S1</f>
+        <v/>
+      </c>
+      <c r="T34">
+        <f>A29*T1</f>
+        <v/>
+      </c>
+      <c r="U34">
+        <f>A29*U1</f>
+        <v/>
+      </c>
+      <c r="V34">
+        <f>A29*V1</f>
+        <v/>
+      </c>
+      <c r="W34">
+        <f>A29*W1</f>
+        <v/>
+      </c>
+      <c r="X34">
+        <f>A29*X1</f>
+        <v/>
+      </c>
+      <c r="Y34">
+        <f>A29*Y1</f>
+        <v/>
+      </c>
+      <c r="Z34">
+        <f>A29*Z1</f>
+        <v/>
+      </c>
+      <c r="AA34">
+        <f>A29*AA1</f>
+        <v/>
+      </c>
+      <c r="AB34">
+        <f>A29*AB1</f>
+        <v/>
+      </c>
+      <c r="AC34">
+        <f>A29*AC1</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:30">
+      <c r="A35" t="n">
         <v>29</v>
       </c>
-      <c r="B32">
+      <c r="B35">
         <f>A30*B1</f>
         <v/>
       </c>
-      <c r="C32">
+      <c r="C35">
         <f>A30*C1</f>
         <v/>
       </c>
-      <c r="D32">
+      <c r="D35">
         <f>A30*D1</f>
         <v/>
       </c>
-      <c r="E32">
+      <c r="E35">
         <f>A30*E1</f>
         <v/>
       </c>
-      <c r="F32">
+      <c r="F35">
         <f>A30*F1</f>
         <v/>
       </c>
-      <c r="G32">
+      <c r="G35">
         <f>A30*G1</f>
         <v/>
       </c>
-      <c r="H32">
+      <c r="H35">
         <f>A30*H1</f>
         <v/>
       </c>
-      <c r="I32">
+      <c r="I35">
         <f>A30*I1</f>
         <v/>
       </c>
-      <c r="J32">
+      <c r="J35">
         <f>A30*J1</f>
         <v/>
       </c>
-      <c r="K32">
+      <c r="K35">
         <f>A30*K1</f>
         <v/>
       </c>
-      <c r="L32">
+      <c r="L35">
         <f>A30*L1</f>
         <v/>
       </c>
-      <c r="M32">
+      <c r="M35">
         <f>A30*M1</f>
         <v/>
       </c>
-      <c r="N32">
+      <c r="N35">
         <f>A30*N1</f>
         <v/>
       </c>
-      <c r="O32">
+      <c r="O35">
         <f>A30*O1</f>
         <v/>
       </c>
-      <c r="P32">
+      <c r="P35">
         <f>A30*P1</f>
         <v/>
       </c>
-      <c r="Q32">
+      <c r="Q35">
         <f>A30*Q1</f>
         <v/>
       </c>
-      <c r="R32">
+      <c r="R35">
         <f>A30*R1</f>
         <v/>
       </c>
-      <c r="S32">
+      <c r="S35">
         <f>A30*S1</f>
         <v/>
       </c>
-      <c r="T32">
+      <c r="T35">
         <f>A30*T1</f>
         <v/>
       </c>
-      <c r="U32">
+      <c r="U35">
         <f>A30*U1</f>
         <v/>
       </c>
-      <c r="V32">
+      <c r="V35">
         <f>A30*V1</f>
         <v/>
       </c>
-      <c r="W32">
+      <c r="W35">
         <f>A30*W1</f>
         <v/>
       </c>
-      <c r="X32">
+      <c r="X35">
         <f>A30*X1</f>
         <v/>
       </c>
-      <c r="Y32">
+      <c r="Y35">
         <f>A30*Y1</f>
         <v/>
       </c>
-      <c r="Z32">
+      <c r="Z35">
         <f>A30*Z1</f>
         <v/>
       </c>
-      <c r="AA32">
+      <c r="AA35">
         <f>A30*AA1</f>
         <v/>
       </c>
-      <c r="AB32">
+      <c r="AB35">
         <f>A30*AB1</f>
         <v/>
       </c>
-      <c r="AC32">
+      <c r="AC35">
         <f>A30*AC1</f>
         <v/>
       </c>

</xml_diff>